<commit_message>
script carga bd completo
</commit_message>
<xml_diff>
--- a/Carga de datos.xlsx
+++ b/Carga de datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manu\Desktop\TrabajoPracticoProgra\TPFinal-e19-Amarilla-Casulo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC61F1B-1B1D-4807-967D-77E447060D9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4BBAFF4-7E83-464D-98F6-89A50385E04F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -883,7 +883,7 @@
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -902,14 +902,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -948,7 +940,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -957,15 +949,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
@@ -1250,8 +1240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O137"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1262,7 +1252,7 @@
     <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.7109375" customWidth="1"/>
     <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="255.5703125" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" customWidth="1"/>
     <col min="13" max="13" width="40" customWidth="1"/>
     <col min="14" max="14" width="22.42578125" customWidth="1"/>
     <col min="16" max="16" width="26.5703125" customWidth="1"/>
@@ -1309,10 +1299,10 @@
       <c r="B2" s="1">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>69</v>
       </c>
       <c r="E2" s="1">
@@ -1324,7 +1314,7 @@
       <c r="G2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2" s="5">
         <v>58650</v>
       </c>
       <c r="I2" s="1">
@@ -1333,9 +1323,9 @@
       <c r="J2" s="1">
         <v>10</v>
       </c>
-      <c r="K2" s="8" t="str">
-        <f>CONCATENATE("INSERT INTO ARTICULOS VALUES ( ",C2, ", ", D2, ", '", E2, "', '", F2, "', '", G2, "', '", H2, "', '", I2, "', '", J2, "');")</f>
-        <v>INSERT INTO ARTICULOS VALUES ( Monitor ASUS 21.5", VP228HE-J Full HD 1ms HDMI VGA, '1', '1', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_27034_Monitor_ASUS_21.5__VP228HE-J_Full_HD_1ms_HDMI_VGA_a797ab9e-grn.jpg', '58650', '1', '10');</v>
+      <c r="K2" s="6" t="str">
+        <f>CONCATENATE("INSERT INTO ARTICULOS VALUES ( '",C2, "', '", D2, "', '", E2, "', '", F2, "', '", G2, "', '", H2, "', '", I2, "', '", J2, "');")</f>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Monitor ASUS 21.5"', 'VP228HE-J Full HD 1ms HDMI VGA', '1', '1', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_27034_Monitor_ASUS_21.5__VP228HE-J_Full_HD_1ms_HDMI_VGA_a797ab9e-grn.jpg', '58650', '1', '10');</v>
       </c>
       <c r="L2">
         <v>1</v>
@@ -1351,15 +1341,15 @@
         <v>INSERT INTO CATEGORIAS (id, descripcion, urlImagen) VALUES ('1', 'Monitores', 'https://cdn-icons-png.flaticon.com/256/81/81793.png');</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1">
         <v>2</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>64</v>
       </c>
       <c r="E3" s="1">
@@ -1371,7 +1361,7 @@
       <c r="G3" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="5">
         <v>119750</v>
       </c>
       <c r="I3" s="1">
@@ -1380,7 +1370,10 @@
       <c r="J3" s="1">
         <v>10</v>
       </c>
-      <c r="K3" s="1"/>
+      <c r="K3" s="6" t="str">
+        <f t="shared" ref="K3:K63" si="0">CONCATENATE("INSERT INTO ARTICULOS VALUES ( '",C3, "', '", D3, "', '", E3, "', '", F3, "', '", G3, "', '", H3, "', '", I3, "', '", J3, "');")</f>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Monitor Gamer MSI 24"', 'Optix G241 144Hz IPS 1ms', '2', '1', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_20990_Monitor_Gamer_MSI_24__Optix_G241_144Hz_IPS_1ms_18f8b03a-grn.jpg', '119750', '1', '10');</v>
+      </c>
       <c r="L3">
         <v>2</v>
       </c>
@@ -1391,19 +1384,19 @@
         <v>39</v>
       </c>
       <c r="O3" t="str">
-        <f t="shared" ref="O3:O11" si="0">CONCATENATE("INSERT INTO CATEGORIAS (id, descripcion, urlImagen) VALUES ('", L3, "', '", M3, "', '", TEXT(N3,"0"), "');")</f>
+        <f t="shared" ref="O3:O11" si="1">CONCATENATE("INSERT INTO CATEGORIAS (id, descripcion, urlImagen) VALUES ('", L3, "', '", M3, "', '", TEXT(N3,"0"), "');")</f>
         <v>INSERT INTO CATEGORIAS (id, descripcion, urlImagen) VALUES ('2', 'Placa de video', 'https://w7.pngwing.com/pngs/388/581/png-transparent-graphics-cards-video-adapters-computer-icons-computer-hardware-electronics-handheld-devices-computer-electronics-text-rectangle-thumbnail.png');</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1">
         <v>3</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="4" t="s">
         <v>77</v>
       </c>
       <c r="E4" s="1">
@@ -1415,7 +1408,7 @@
       <c r="G4" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="5">
         <v>77900</v>
       </c>
       <c r="I4" s="1">
@@ -1424,7 +1417,10 @@
       <c r="J4" s="1">
         <v>10</v>
       </c>
-      <c r="K4" s="1"/>
+      <c r="K4" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Monitor ASUS 24"', 'VA24EHE-J Full HD', '1', '1', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_33878_Monitor_ASUS_24__VA24EHE-J_Full_HD_ac877e59-grn.jpg', '77900', '1', '10');</v>
+      </c>
       <c r="L4">
         <v>3</v>
       </c>
@@ -1435,19 +1431,19 @@
         <v>40</v>
       </c>
       <c r="O4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO CATEGORIAS (id, descripcion, urlImagen) VALUES ('3', 'Disco Solido', 'https://cdn-icons-png.flaticon.com/256/4400/4400889.png');</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1">
         <v>4</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="4" t="s">
         <v>79</v>
       </c>
       <c r="E5" s="1">
@@ -1459,7 +1455,7 @@
       <c r="G5" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="5">
         <v>60000</v>
       </c>
       <c r="I5" s="1">
@@ -1468,7 +1464,10 @@
       <c r="J5" s="1">
         <v>10</v>
       </c>
-      <c r="K5" s="1"/>
+      <c r="K5" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Monitor ASUS 27"', ' Full HD HDMI VGA VA27EHE-J', '1', '1', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_33822_Monitor_ASUS_27__Full_HD_HDMI_VGA_VA27EHE-J_8b229ce8-grn.jpg', '60000', '1', '10');</v>
+      </c>
       <c r="L5">
         <v>4</v>
       </c>
@@ -1479,19 +1478,19 @@
         <v>41</v>
       </c>
       <c r="O5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO CATEGORIAS (id, descripcion, urlImagen) VALUES ('4', 'Disco rígido', 'https://e7.pngegg.com/pngimages/605/607/png-clipart-logo-brand-data-font-hard-disc-icon-text-rectangle-thumbnail.png');</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1">
         <v>5</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="4" t="s">
         <v>52</v>
       </c>
       <c r="E6" s="1">
@@ -1503,7 +1502,7 @@
       <c r="G6" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="5">
         <v>111500</v>
       </c>
       <c r="I6" s="1">
@@ -1512,7 +1511,10 @@
       <c r="J6" s="1">
         <v>10</v>
       </c>
-      <c r="K6" s="1"/>
+      <c r="K6" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Monitor Gamer Viewsonic 24"', ' VX2468-PC-MHD Curvo 165hz', '11', '1', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_33359_Monitor_Gamer_Viewsonic_24__VX2468-PC-MHD_Curvo_165hz_46d27d6d-grn.jpg', '111500', '1', '10');</v>
+      </c>
       <c r="L6">
         <v>5</v>
       </c>
@@ -1523,19 +1525,19 @@
         <v>42</v>
       </c>
       <c r="O6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO CATEGORIAS (id, descripcion, urlImagen) VALUES ('5', 'Memoria Ram', 'https://cdn-icons-png.flaticon.com/256/882/882566.png');</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1">
         <v>6</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="4" t="s">
         <v>58</v>
       </c>
       <c r="E7" s="1">
@@ -1547,7 +1549,7 @@
       <c r="G7" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="5">
         <v>207300</v>
       </c>
       <c r="I7" s="1">
@@ -1556,7 +1558,10 @@
       <c r="J7" s="1">
         <v>10</v>
       </c>
-      <c r="K7" s="1"/>
+      <c r="K7" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Monitor Gamer Viewsonic 27"', 'VX2768 Curvo 2K 144Hz 1ms FreeSync HDMI DP', '11', '1', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_23822_Monitor_Gamer_Viewsonic_27__VX2768_Curvo_2K_144Hz_1ms_FreeSync_HDMI_DP_071c1138-grn.jpg', '207300', '1', '10');</v>
+      </c>
       <c r="L7">
         <v>6</v>
       </c>
@@ -1567,11 +1572,11 @@
         <v>43</v>
       </c>
       <c r="O7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO CATEGORIAS (id, descripcion, urlImagen) VALUES ('6', 'Teclado', 'https://cdn-icons-png.flaticon.com/256/5740/5740915.png');</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>7</v>
       </c>
@@ -1590,7 +1595,7 @@
       <c r="G8" t="s">
         <v>83</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="5">
         <v>443650</v>
       </c>
       <c r="I8" s="1">
@@ -1598,6 +1603,10 @@
       </c>
       <c r="J8" s="1">
         <v>10</v>
+      </c>
+      <c r="K8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Placa de Video MSI GeForce RTX 3090', '24GB GDDR6X VENTUS 3X OC', '2', '2', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_36639_Placa_de_Video_MSI_GeForce_RTX_3090_24GB_GDDR6X_VENTUS_3X_OC_58618d16-grn.jpg', '443650', '1', '10');</v>
       </c>
       <c r="L8">
         <v>7</v>
@@ -1609,11 +1618,11 @@
         <v>44</v>
       </c>
       <c r="O8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO CATEGORIAS (id, descripcion, urlImagen) VALUES ('7', 'Mouse', 'https://i.pinimg.com/originals/e9/09/ea/e909ea4f8dff04c13c36d9856a977ebd.png');</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B9" s="1">
         <v>8</v>
       </c>
@@ -1632,7 +1641,7 @@
       <c r="G9" t="s">
         <v>90</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="5">
         <v>130000</v>
       </c>
       <c r="I9" s="1">
@@ -1640,6 +1649,10 @@
       </c>
       <c r="J9" s="1">
         <v>10</v>
+      </c>
+      <c r="K9" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Placa de Video ASUS Phoenix GeForce GTX 1630', '4GB GDDR6', '1', '2', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_36550_Placa_de_Video_ASUS_Phoenix_GeForce_GTX_1630_4GB_GDDR6_b0a0edd2-grn.jpg', '130000', '1', '10');</v>
       </c>
       <c r="L9">
         <v>8</v>
@@ -1651,11 +1664,11 @@
         <v>45</v>
       </c>
       <c r="O9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO CATEGORIAS (id, descripcion, urlImagen) VALUES ('8', 'Auriculares', 'https://cdn-icons-png.flaticon.com/256/260/260315.png');</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B10" s="1">
         <v>9</v>
       </c>
@@ -1674,7 +1687,7 @@
       <c r="G10" t="s">
         <v>94</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="5">
         <v>205000</v>
       </c>
       <c r="I10" s="1">
@@ -1682,6 +1695,10 @@
       </c>
       <c r="J10" s="1">
         <v>10</v>
+      </c>
+      <c r="K10" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Placa de Video ASUS GeForce GTX 1660 SUPER', '6GB GDDR6 OC TUF', '1', '2', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_35211_Placa_de_Video_ASUS_GeForce_GTX_1660_SUPER_6GB_GDDR6_OC_TUF_91e6cd72-grn.jpg', '205000', '1', '10');</v>
       </c>
       <c r="L10">
         <v>9</v>
@@ -1693,11 +1710,11 @@
         <v>46</v>
       </c>
       <c r="O10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO CATEGORIAS (id, descripcion, urlImagen) VALUES ('9', 'Placa madre', 'https://cdn-icons-png.flaticon.com/256/2004/2004686.png');</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B11" s="1">
         <v>10</v>
       </c>
@@ -1716,7 +1733,7 @@
       <c r="G11" t="s">
         <v>99</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="5">
         <v>190000</v>
       </c>
       <c r="I11" s="1">
@@ -1724,6 +1741,10 @@
       </c>
       <c r="J11" s="1">
         <v>10</v>
+      </c>
+      <c r="K11" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Placa de Video ASUS GeForce GTX 1650', '4GB GDDR6 TUF GAMING', '1', '2', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_27548_Placa_de_Video_ASUS_GeForce_GTX_1650_4GB_GDDR6_TUF_GAMING_71e82ff4-grn.jpg', '190000', '1', '10');</v>
       </c>
       <c r="L11">
         <v>10</v>
@@ -1735,11 +1756,11 @@
         <v>47</v>
       </c>
       <c r="O11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO CATEGORIAS (id, descripcion, urlImagen) VALUES ('10', 'Procesador', 'https://cdn-icons-png.flaticon.com/256/1086/1086611.png');</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B12" s="1">
         <v>11</v>
       </c>
@@ -1758,7 +1779,7 @@
       <c r="G12" t="s">
         <v>105</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12" s="5">
         <v>58000</v>
       </c>
       <c r="I12" s="1">
@@ -1767,8 +1788,12 @@
       <c r="J12" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K12" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Placa de Video Asrock Radeon RX 550', '2GB GDDR5 Phantom Gaming', '11', '2', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_19289_Placa_de_Video_Asrock_Radeon_RX_550_2GB_GDDR5_Phantom_Gaming_99528ce8-grn.jpg', '58000', '1', '10');</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
         <v>12</v>
       </c>
@@ -1787,7 +1812,7 @@
       <c r="G13" t="s">
         <v>109</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H13" s="5">
         <v>283000</v>
       </c>
       <c r="I13" s="1">
@@ -1796,9 +1821,12 @@
       <c r="J13" s="1">
         <v>10</v>
       </c>
-      <c r="K13" s="4"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K13" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Placa de Video Asrock Radeon RX 6800', 'XT 16GB GDDR6 Phantom Gaming D OC', '11', '2', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_29154_Placa_de_Video_Asrock_Radeon_RX_6800_XT_16GB_GDDR6_Phantom_Gaming_D_OC_b76349fe-grn.jpg', '283000', '1', '10');</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B14" s="1">
         <v>13</v>
       </c>
@@ -1817,7 +1845,7 @@
       <c r="G14" t="s">
         <v>114</v>
       </c>
-      <c r="H14" s="7">
+      <c r="H14" s="5">
         <v>27000</v>
       </c>
       <c r="I14" s="1">
@@ -1825,19 +1853,23 @@
       </c>
       <c r="J14" s="1">
         <v>10</v>
+      </c>
+      <c r="K14" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Disco Solido SSD M.2 WD 500GB Blue', 'SN570 3500MB/s NVMe PCI-E Gen3 x4 TLC', '9', '3', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_32107_Disco_Solido_SSD_M.2_WD_500GB_Blue_SN570_3500MB_s_NVMe_PCI-E_Gen3_x4_TLC_3135e1e9-grn.jpg', '27000', '1', '10');</v>
       </c>
       <c r="M14" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B15" s="1">
         <v>14</v>
       </c>
       <c r="C15" t="s">
         <v>116</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" t="s">
         <v>117</v>
       </c>
       <c r="E15" s="1">
@@ -1849,7 +1881,7 @@
       <c r="G15" t="s">
         <v>118</v>
       </c>
-      <c r="H15" s="7">
+      <c r="H15" s="5">
         <v>31000</v>
       </c>
       <c r="I15" s="1">
@@ -1857,6 +1889,10 @@
       </c>
       <c r="J15" s="1">
         <v>10</v>
+      </c>
+      <c r="K15" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Disco Solido SSD M.2 WD 500GB Black', 'SN750 SE 3600MB/s PCI-E X4 NVMe GEN4', '9', '3', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_28600_Disco_Solido_SSD_M.2_WD_500GB_Black_SN750_SE_3600MB_s_PCI-E_X4_NVMe_GEN4_b815bec0-grn.jpg', '31000', '1', '10');</v>
       </c>
       <c r="L15">
         <v>1</v>
@@ -1872,7 +1908,7 @@
         <v>INSERT INTO MARCAS (id, descripcion, urlImagen) VALUES ('1', 'Asus', 'https://images.freeimages.com/fic/images/icons/2796/metro_uinvert_dock/256/asus.png');</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B16" s="1">
         <v>15</v>
       </c>
@@ -1891,7 +1927,7 @@
       <c r="G16" t="s">
         <v>122</v>
       </c>
-      <c r="H16" s="7">
+      <c r="H16" s="5">
         <v>42300</v>
       </c>
       <c r="I16" s="1">
@@ -1899,6 +1935,10 @@
       </c>
       <c r="J16" s="1">
         <v>10</v>
+      </c>
+      <c r="K16" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Disco Solido SSD M.2 WD 500GB WD_Black', 'SN770 5000MB/s NVMe PCI-E x4 Gen 4', '9', '3', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_33159_Disco_Solido_SSD_M.2_WD_500GB_WD_Black_SN770_5000MB_s_NVMe_PCI-E_x4_Gen_4_7a4a307b-grn.jpg', '42300', '1', '10');</v>
       </c>
       <c r="L16">
         <v>2</v>
@@ -1910,11 +1950,11 @@
         <v>36</v>
       </c>
       <c r="O16" t="str">
-        <f t="shared" ref="O16:O26" si="1">CONCATENATE("INSERT INTO MARCAS (id, descripcion, urlImagen) VALUES ('", L16, "', '", M16, "', '", TEXT(N16,"0"), "');")</f>
+        <f t="shared" ref="O16:O26" si="2">CONCATENATE("INSERT INTO MARCAS (id, descripcion, urlImagen) VALUES ('", L16, "', '", M16, "', '", TEXT(N16,"0"), "');")</f>
         <v>INSERT INTO MARCAS (id, descripcion, urlImagen) VALUES ('2', 'MSI', 'https://pbs.twimg.com/profile_images/674660612547432448/-mac6Il7_400x400.jpg');</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:15" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B17" s="1">
         <v>16</v>
       </c>
@@ -1933,7 +1973,7 @@
       <c r="G17" t="s">
         <v>126</v>
       </c>
-      <c r="H17" s="7">
+      <c r="H17" s="5">
         <v>69000</v>
       </c>
       <c r="I17" s="1">
@@ -1941,6 +1981,10 @@
       </c>
       <c r="J17" s="1">
         <v>10</v>
+      </c>
+      <c r="K17" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Disco Solido SSD M.2 WD 1TB WD_Black SN770', '5150MB/s NVMe PCI-E x4 Gen 4', '9', '3', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_35589_Disco_Solido_SSD_M.2_WD_1TB_WD_Black_SN770_5150MB_s_NVMe_PCI-E_x4_Gen_4_7a4a307b-grn.jpg', '69000', '1', '10');</v>
       </c>
       <c r="L17">
         <v>3</v>
@@ -1952,11 +1996,11 @@
         <v>30</v>
       </c>
       <c r="O17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>INSERT INTO MARCAS (id, descripcion, urlImagen) VALUES ('3', 'Amd', 'https://compragamer.net/imagenes_marcas/imagen_marca_320_9_411.jpg');</v>
       </c>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:15" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B18" s="1">
         <v>17</v>
       </c>
@@ -1975,7 +2019,7 @@
       <c r="G18" t="s">
         <v>130</v>
       </c>
-      <c r="H18" s="7">
+      <c r="H18" s="5">
         <v>14000</v>
       </c>
       <c r="I18" s="1">
@@ -1983,6 +2027,10 @@
       </c>
       <c r="J18" s="1">
         <v>10</v>
+      </c>
+      <c r="K18" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Disco Solido SSD Adata 240GB', 'SU650SS 520MB/s*', '12', '3', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_29777_Disco_Solido_SSD_Adata_240GB_SU650SS_520MB_s__8b455937-grn.jpg', '14000', '1', '10');</v>
       </c>
       <c r="L18">
         <v>4</v>
@@ -1994,11 +2042,11 @@
         <v>29</v>
       </c>
       <c r="O18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>INSERT INTO MARCAS (id, descripcion, urlImagen) VALUES ('4', 'Intel', 'https://compragamer.net/imagenes_marcas/imagen_marca_364_9_203.jpg');</v>
       </c>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:15" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B19" s="1">
         <v>18</v>
       </c>
@@ -2017,7 +2065,7 @@
       <c r="G19" t="s">
         <v>134</v>
       </c>
-      <c r="H19" s="7">
+      <c r="H19" s="5">
         <v>22000</v>
       </c>
       <c r="I19" s="1">
@@ -2025,6 +2073,10 @@
       </c>
       <c r="J19" s="1">
         <v>10</v>
+      </c>
+      <c r="K19" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Disco Rígido WD 1TB BLUE', '64MB SATA 6.0GB/s ', '9', '4', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_9018_Disco_R__gido_WD_1TB_BLUE_64MB_SATA_6.0GB_s__ca74d162-grn.jpg', '22000', '1', '10');</v>
       </c>
       <c r="L19">
         <v>5</v>
@@ -2036,11 +2088,11 @@
         <v>37</v>
       </c>
       <c r="O19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>INSERT INTO MARCAS (id, descripcion, urlImagen) VALUES ('5', 'Logitech', 'https://static.macupdate.com/products/62352/l/logitech-g-hub-logo.webp?v=1671137096');</v>
       </c>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:15" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B20" s="1">
         <v>19</v>
       </c>
@@ -2059,7 +2111,7 @@
       <c r="G20" t="s">
         <v>138</v>
       </c>
-      <c r="H20" s="7">
+      <c r="H20" s="5">
         <v>34000</v>
       </c>
       <c r="I20" s="1">
@@ -2067,6 +2119,10 @@
       </c>
       <c r="J20" s="1">
         <v>10</v>
+      </c>
+      <c r="K20" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Disco Rigido WD 2TB BLUE', '256MB SATA 6.0GB/s', '9', '4', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_21014_Disco_Rigido_WD_2TB_BLUE_256MB_SATA_6.0GB_s_44f766ac-grn.jpg', '34000', '1', '10');</v>
       </c>
       <c r="L20">
         <v>6</v>
@@ -2078,11 +2134,11 @@
         <v>33</v>
       </c>
       <c r="O20" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>INSERT INTO MARCAS (id, descripcion, urlImagen) VALUES ('6', 'Redragon', 'https://styles.redditmedia.com/t5_42nhxk/styles/communityIcon_vb8305k77xo61.png?width=256&amp;s=7a4a763b7f929dd1ee7fe6ea04f9a27d71c581e0');</v>
       </c>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:15" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B21" s="1">
         <v>20</v>
       </c>
@@ -2101,7 +2157,7 @@
       <c r="G21" t="s">
         <v>141</v>
       </c>
-      <c r="H21" s="7">
+      <c r="H21" s="5">
         <v>34000</v>
       </c>
       <c r="I21" s="1">
@@ -2109,6 +2165,10 @@
       </c>
       <c r="J21" s="1">
         <v>10</v>
+      </c>
+      <c r="K21" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Disco Rigido WD 2TB BLUE', '256MB SATA 6.0GB/s 7200RPM', '9', '4', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_35996_Disco_Rigido_WD_2TB_BLUE_256MB_SATA_6.0GB_s_7200RPM_dc36f8f5-grn.jpg', '34000', '1', '10');</v>
       </c>
       <c r="L21">
         <v>7</v>
@@ -2120,11 +2180,11 @@
         <v>31</v>
       </c>
       <c r="O21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>INSERT INTO MARCAS (id, descripcion, urlImagen) VALUES ('7', 'HyperX', 'https://compragamer.net/imagenes_marcas/imagen_marca_365_9_441.jpg');</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:15" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B22" s="1">
         <v>21</v>
       </c>
@@ -2143,7 +2203,7 @@
       <c r="G22" t="s">
         <v>144</v>
       </c>
-      <c r="H22" s="7">
+      <c r="H22" s="5">
         <v>126000</v>
       </c>
       <c r="I22" s="1">
@@ -2151,6 +2211,10 @@
       </c>
       <c r="J22" s="1">
         <v>10</v>
+      </c>
+      <c r="K22" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Disco Rigido WD 12TB Red', 'Pro 7.2K RPM 256MB', '9', '4', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_26480_Disco_Rigido_WD_12TB_Red_Pro_7.2K_RPM_256MB_c66a3fa3-grn.jpg', '126000', '1', '10');</v>
       </c>
       <c r="L22">
         <v>8</v>
@@ -2162,11 +2226,11 @@
         <v>34</v>
       </c>
       <c r="O22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>INSERT INTO MARCAS (id, descripcion, urlImagen) VALUES ('8', 'Genius', 'https://www.lacasadelacomputadora.com.uy/imgs/representaciones/foto31_71.jpg');</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:15" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B23" s="1">
         <v>22</v>
       </c>
@@ -2185,7 +2249,7 @@
       <c r="G23" t="s">
         <v>147</v>
       </c>
-      <c r="H23" s="7">
+      <c r="H23" s="5">
         <v>128000</v>
       </c>
       <c r="I23" s="1">
@@ -2193,6 +2257,10 @@
       </c>
       <c r="J23" s="1">
         <v>10</v>
+      </c>
+      <c r="K23" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Disco Rigido WD 12TB Gold', '7.2K RPM 256MB', '9', '4', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_26484_Disco_Rigido_WD_12TB_Gold_7.2K_RPM_256MB_856fe552-grn.jpg', '128000', '1', '10');</v>
       </c>
       <c r="L23">
         <v>9</v>
@@ -2204,11 +2272,11 @@
         <v>32</v>
       </c>
       <c r="O23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>INSERT INTO MARCAS (id, descripcion, urlImagen) VALUES ('9', 'Western Digital', 'https://compragamer.net/imagenes_marcas/imagen_marca_322_9_619.jpg');</v>
       </c>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:15" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B24" s="1">
         <v>23</v>
       </c>
@@ -2227,7 +2295,7 @@
       <c r="G24" t="s">
         <v>152</v>
       </c>
-      <c r="H24" s="7">
+      <c r="H24" s="5">
         <v>10500</v>
       </c>
       <c r="I24" s="1">
@@ -2235,6 +2303,10 @@
       </c>
       <c r="J24" s="1">
         <v>10</v>
+      </c>
+      <c r="K24" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Memoria Adata DDR4 4GB', ' 2666MHz Value ', '12', '5', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_13221_Memoria_Adata_DDR4_4GB_2666MHz_Value__aa6df289-grn.jpg', '10500', '1', '10');</v>
       </c>
       <c r="L24">
         <v>10</v>
@@ -2246,11 +2318,11 @@
         <v>49</v>
       </c>
       <c r="O24" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>INSERT INTO MARCAS (id, descripcion, urlImagen) VALUES ('10', 'ViewSonic', 'https://e7.pngegg.com/pngimages/466/107/png-clipart-hewlett-packard-viewsonic-computer-monitors-logo-computer-software-hewlett-packard-text-logo.png');</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:15" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B25" s="1">
         <v>24</v>
       </c>
@@ -2269,7 +2341,7 @@
       <c r="G25" t="s">
         <v>155</v>
       </c>
-      <c r="H25" s="7">
+      <c r="H25" s="5">
         <v>17000</v>
       </c>
       <c r="I25" s="1">
@@ -2277,6 +2349,10 @@
       </c>
       <c r="J25" s="1">
         <v>10</v>
+      </c>
+      <c r="K25" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Memoria Adata DDR4 8GB ', ' 2666MHz Value Sodimm Notebook', '12', '5', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_16184_Memoria_Adata_DDR4_8GB_2666MHz_Value_Sodimm_Notebook_38c2e2af-grn.jpg', '17000', '1', '10');</v>
       </c>
       <c r="L25">
         <v>11</v>
@@ -2288,11 +2364,11 @@
         <v>102</v>
       </c>
       <c r="O25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>INSERT INTO MARCAS (id, descripcion, urlImagen) VALUES ('11', 'Asrock', 'https://cdn.shopify.com/s/files/1/0331/2789/1082/products/ASRock_grande.jpg?v=1582152086');</v>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:15" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B26" s="1">
         <v>25</v>
       </c>
@@ -2311,7 +2387,7 @@
       <c r="G26" t="s">
         <v>158</v>
       </c>
-      <c r="H26" s="7">
+      <c r="H26" s="5">
         <v>19500</v>
       </c>
       <c r="I26" s="1">
@@ -2319,6 +2395,10 @@
       </c>
       <c r="J26" s="1">
         <v>10</v>
+      </c>
+      <c r="K26" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Memoria Adata DDR4 8GB', '3200MHz Premier', '12', '5', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_18814_Memoria_Adata_DDR4_8GB_3200MHz_Premier_c6036c27-grn.jpg', '19500', '1', '10');</v>
       </c>
       <c r="L26">
         <v>12</v>
@@ -2330,11 +2410,11 @@
         <v>149</v>
       </c>
       <c r="O26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>INSERT INTO MARCAS (id, descripcion, urlImagen) VALUES ('12', 'Adata', 'https://2.bp.blogspot.com/-yTiEnencHOA/T08JEEqNlKI/AAAAAAAABts/luVxNynFvW8/s1600/a6.jpg');</v>
       </c>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:15" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B27" s="1">
         <v>26</v>
       </c>
@@ -2353,7 +2433,7 @@
       <c r="G27" t="s">
         <v>159</v>
       </c>
-      <c r="H27" s="7">
+      <c r="H27" s="5">
         <v>43000</v>
       </c>
       <c r="I27" s="1">
@@ -2362,8 +2442,12 @@
       <c r="J27" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="K27" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Memoria Adata DDR4 16GB', '3200MHz CL16 XPG GAMMIX D20 Black', '12', '5', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_25890_Memoria_Adata_DDR4_16GB_3200MHz_CL16_XPG_GAMMIX_D20_Black_6b1582d3-grn.jpg', '43000', '1', '10');</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B28" s="1">
         <v>27</v>
       </c>
@@ -2382,7 +2466,7 @@
       <c r="G28" t="s">
         <v>163</v>
       </c>
-      <c r="H28" s="7">
+      <c r="H28" s="5">
         <v>21200</v>
       </c>
       <c r="I28" s="1">
@@ -2391,8 +2475,12 @@
       <c r="J28" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="K28" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Memoria Adata DDR4 8GB ', '3200MHz XPG Spectrix D60G RGB Titanium', '12', '5', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_28924_Memoria_Adata_DDR4_8GB_3200MHz_XPG_Spectrix_D60G_RGB_Titanium_88f51e0f-grn.jpg', '21200', '1', '10');</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B29" s="1">
         <v>28</v>
       </c>
@@ -2411,7 +2499,7 @@
       <c r="G29" t="s">
         <v>165</v>
       </c>
-      <c r="H29" s="7">
+      <c r="H29" s="5">
         <v>25000</v>
       </c>
       <c r="I29" s="1">
@@ -2419,12 +2507,16 @@
       </c>
       <c r="J29" s="1">
         <v>10</v>
+      </c>
+      <c r="K29" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Memoria Adata DDR4 8GB', '3200MHz XPG Spectrix D50 RGB Titanium', '12', '5', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_28926_Memoria_Adata_DDR4_8GB_3200MHz_XPG_Spectrix_D50_RGB_Titanium_446ebe28-grn.jpg', '25000', '1', '10');</v>
       </c>
       <c r="M29" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:15" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B30" s="1">
         <v>29</v>
       </c>
@@ -2443,7 +2535,7 @@
       <c r="G30" t="s">
         <v>168</v>
       </c>
-      <c r="H30" s="7">
+      <c r="H30" s="5">
         <v>340000</v>
       </c>
       <c r="I30" s="1">
@@ -2451,6 +2543,10 @@
       </c>
       <c r="J30" s="1">
         <v>10</v>
+      </c>
+      <c r="K30" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Memoria Adata DDR4 (2x8GB) 16GB ', '5000MHz XPG Spectrix D50 Xtreme RGB CL19', '12', '5', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_29885_Memoria_Adata_DDR4__2x8GB__16GB_5000MHz_XPG_Spectrix_D50_Xtreme_RGB_CL19_18133a6d-grn.jpg', '340000', '1', '10');</v>
       </c>
       <c r="L30">
         <v>5</v>
@@ -2463,7 +2559,7 @@
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('5','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_33359_Monitor_Gamer_Viewsonic_24__VX2468-PC-MHD_Curvo_165hz_46d27d6d-grn.jpg');</v>
       </c>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:15" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B31" s="1">
         <v>30</v>
       </c>
@@ -2482,7 +2578,7 @@
       <c r="G31" t="s">
         <v>170</v>
       </c>
-      <c r="H31" s="7">
+      <c r="H31" s="5">
         <v>24500</v>
       </c>
       <c r="I31" s="1">
@@ -2490,6 +2586,10 @@
       </c>
       <c r="J31" s="1">
         <v>10</v>
+      </c>
+      <c r="K31" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Memoria Adata DDR4 8GB', '3600Mhz XPG Spectrix D45G RGB', '12', '5', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_29565_Memoria_Adata_DDR4_8GB_3600Mhz_XPG_Spectrix_D45G_RGB_cbbc726d-grn.jpg', '24500', '1', '10');</v>
       </c>
       <c r="L31">
         <v>5</v>
@@ -2498,18 +2598,18 @@
         <v>55</v>
       </c>
       <c r="N31" t="str">
-        <f t="shared" ref="N31:N94" si="2">CONCATENATE("INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('", L31, "','", TEXT(M31,"0"), "');")</f>
+        <f t="shared" ref="N31:N94" si="3">CONCATENATE("INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('", L31, "','", TEXT(M31,"0"), "');")</f>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('5','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_33360_Monitor_Gamer_Viewsonic_24__VX2468-PC-MHD_Curvo_165hz_a6deb2ae-grn.jpg');</v>
       </c>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:15" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B32" s="1">
         <v>31</v>
       </c>
       <c r="C32" t="s">
         <v>171</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" t="s">
         <v>172</v>
       </c>
       <c r="E32" s="1">
@@ -2521,7 +2621,7 @@
       <c r="G32" t="s">
         <v>173</v>
       </c>
-      <c r="H32" s="7">
+      <c r="H32" s="5">
         <v>39000</v>
       </c>
       <c r="I32" s="1">
@@ -2529,6 +2629,10 @@
       </c>
       <c r="J32" s="1">
         <v>10</v>
+      </c>
+      <c r="K32" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Teclado Mecanico Logitech PRO TKL', 'LOL 2 Switch Brown', '5', '6', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_33275_Teclado_Mecanico_Logitech_PRO_TKL_LOL_2_Switch_Brown_30e10b48-grn.jpg', '39000', '1', '10');</v>
       </c>
       <c r="L32">
         <v>5</v>
@@ -2537,11 +2641,11 @@
         <v>56</v>
       </c>
       <c r="N32" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('5','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_33362_Monitor_Gamer_Viewsonic_24__VX2468-PC-MHD_Curvo_165hz_ac523dc3-grn.jpg');</v>
       </c>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B33" s="1">
         <v>32</v>
       </c>
@@ -2560,7 +2664,7 @@
       <c r="G33" t="s">
         <v>176</v>
       </c>
-      <c r="H33" s="7">
+      <c r="H33" s="5">
         <v>50000</v>
       </c>
       <c r="I33" s="1">
@@ -2568,6 +2672,10 @@
       </c>
       <c r="J33" s="1">
         <v>10</v>
+      </c>
+      <c r="K33" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Teclado Mecanico Logitech G513', 'Carbon RGB Switch GX Brown Español', '5', '6', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_19865_Teclado_Mecanico_Logitech_G513_Carbon_RGB_Switch_GX_Brown_Espa__ol_9ccf7c47-grn.jpg', '50000', '1', '10');</v>
       </c>
       <c r="L33">
         <v>6</v>
@@ -2576,11 +2684,11 @@
         <v>60</v>
       </c>
       <c r="N33" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('6','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_23821_Monitor_Gamer_Viewsonic_27__VX2768_Curvo_2K_144Hz_1ms_FreeSync_HDMI_DP_af5acee2-grn.jpg');</v>
       </c>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B34" s="1">
         <v>33</v>
       </c>
@@ -2599,7 +2707,7 @@
       <c r="G34" t="s">
         <v>179</v>
       </c>
-      <c r="H34" s="7">
+      <c r="H34" s="5">
         <v>52200</v>
       </c>
       <c r="I34" s="1">
@@ -2607,6 +2715,10 @@
       </c>
       <c r="J34" s="1">
         <v>10</v>
+      </c>
+      <c r="K34" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Teclado Mecanico Logitech POP Blast', 'Yellow Wireless', '5', '6', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_33269_Teclado_Mecanico_Logitech_POP_Blast_Yellow_Wireless_725996a0-grn.jpg', '52200', '1', '10');</v>
       </c>
       <c r="L34">
         <v>6</v>
@@ -2615,11 +2727,11 @@
         <v>61</v>
       </c>
       <c r="N34" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('6','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_23823_Monitor_Gamer_Viewsonic_27__VX2768_Curvo_2K_144Hz_1ms_FreeSync_HDMI_DP_428c53c0-grn.jpg');</v>
       </c>
     </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B35" s="1">
         <v>34</v>
       </c>
@@ -2638,7 +2750,7 @@
       <c r="G35" t="s">
         <v>182</v>
       </c>
-      <c r="H35" s="7">
+      <c r="H35" s="5">
         <v>52000</v>
       </c>
       <c r="I35" s="1">
@@ -2646,6 +2758,10 @@
       </c>
       <c r="J35" s="1">
         <v>10</v>
+      </c>
+      <c r="K35" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Teclado Mecanico Logitech POP', 'Coral Rose Wireless', '5', '6', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_36665_Teclado_Mecanico_Logitech_POP_Coral_Rose_Wireless_065ab138-grn.jpg', '52000', '1', '10');</v>
       </c>
       <c r="L35">
         <v>2</v>
@@ -2654,11 +2770,11 @@
         <v>65</v>
       </c>
       <c r="N35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('2','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_20991_Monitor_Gamer_MSI_24__Optix_G241_144Hz_IPS_1ms_204c32c9-grn.jpg');</v>
       </c>
     </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B36" s="1">
         <v>35</v>
       </c>
@@ -2677,7 +2793,7 @@
       <c r="G36" t="s">
         <v>185</v>
       </c>
-      <c r="H36" s="7">
+      <c r="H36" s="5">
         <v>88000</v>
       </c>
       <c r="I36" s="1">
@@ -2685,6 +2801,10 @@
       </c>
       <c r="J36" s="1">
         <v>10</v>
+      </c>
+      <c r="K36" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Teclado Logitech G815', 'Mechanical RGB Lightsync', '5', '6', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_16207_Teclado_Logitech_G815_Mechanical_RGB_Lightsync_5ab9b8b1-grn.jpg', '88000', '1', '10');</v>
       </c>
       <c r="L36">
         <v>2</v>
@@ -2693,11 +2813,11 @@
         <v>66</v>
       </c>
       <c r="N36" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('2','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_20992_Monitor_Gamer_MSI_24__Optix_G241_144Hz_IPS_1ms_4be4b651-grn.jpg');</v>
       </c>
     </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B37" s="1">
         <v>36</v>
       </c>
@@ -2716,7 +2836,7 @@
       <c r="G37" t="s">
         <v>188</v>
       </c>
-      <c r="H37" s="7">
+      <c r="H37" s="5">
         <v>115000</v>
       </c>
       <c r="I37" s="1">
@@ -2724,6 +2844,10 @@
       </c>
       <c r="J37" s="1">
         <v>10</v>
+      </c>
+      <c r="K37" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Teclado Mecanico Logitech G915 TKL', 'RGB Lightspeed Inalambrico', '5', '6', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_19373_Teclado_Mecanico_Logitech_G915_TKL_RGB_Lightspeed_Inalambrico_065f0cec-grn.jpg', '115000', '1', '10');</v>
       </c>
       <c r="L37">
         <v>2</v>
@@ -2732,11 +2856,11 @@
         <v>67</v>
       </c>
       <c r="N37" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('2','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_20993_Monitor_Gamer_MSI_24__Optix_G241_144Hz_IPS_1ms_3a4c4094-grn.jpg');</v>
       </c>
     </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B38" s="1">
         <v>37</v>
       </c>
@@ -2752,7 +2876,7 @@
       <c r="F38" s="1">
         <v>6</v>
       </c>
-      <c r="H38" s="7">
+      <c r="H38" s="5">
         <v>119000</v>
       </c>
       <c r="I38" s="1">
@@ -2760,6 +2884,10 @@
       </c>
       <c r="J38" s="1">
         <v>10</v>
+      </c>
+      <c r="K38" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Teclado Mecanico Logitech Aurora G715', 'Wireless White RGB', '5', '6', '', '119000', '1', '10');</v>
       </c>
       <c r="L38">
         <v>1</v>
@@ -2768,11 +2896,11 @@
         <v>71</v>
       </c>
       <c r="N38" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('1','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_27036_Monitor_ASUS_21.5__VP228HE-J_Full_HD_1ms_HDMI_VGA_29ad25c0-grn.jpg');</v>
       </c>
     </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B39" s="1">
         <v>38</v>
       </c>
@@ -2791,7 +2919,7 @@
       <c r="G39" t="s">
         <v>193</v>
       </c>
-      <c r="H39" s="7">
+      <c r="H39" s="5">
         <v>7300</v>
       </c>
       <c r="I39" s="1">
@@ -2799,6 +2927,10 @@
       </c>
       <c r="J39" s="1">
         <v>10</v>
+      </c>
+      <c r="K39" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Mouse Redragon Centrophorus ', 'M601 RGB', '6', '7', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_28612_Mouse_Redragon_Centrophorus_M601_RGB_e00743a5-grn.jpg', '7300', '1', '10');</v>
       </c>
       <c r="L39">
         <v>1</v>
@@ -2807,11 +2939,11 @@
         <v>72</v>
       </c>
       <c r="N39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('1','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_27037_Monitor_ASUS_21.5__VP228HE-J_Full_HD_1ms_HDMI_VGA_313cf0e0-med.jpg');</v>
       </c>
     </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B40" s="1">
         <v>39</v>
       </c>
@@ -2830,7 +2962,7 @@
       <c r="G40" t="s">
         <v>197</v>
       </c>
-      <c r="H40" s="7">
+      <c r="H40" s="5">
         <v>7500</v>
       </c>
       <c r="I40" s="1">
@@ -2838,6 +2970,10 @@
       </c>
       <c r="J40" s="1">
         <v>10</v>
+      </c>
+      <c r="K40" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Mouse Redragon Mirage M690', '2.5GHz Wireless', '6', '7', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_8760_Mouse_Redragon_Mirage_M690_2.5GHz_Wireless_1739dc55-grn.jpg', '7500', '1', '10');</v>
       </c>
       <c r="L40">
         <v>1</v>
@@ -2846,11 +2982,11 @@
         <v>71</v>
       </c>
       <c r="N40" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('1','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_27036_Monitor_ASUS_21.5__VP228HE-J_Full_HD_1ms_HDMI_VGA_29ad25c0-grn.jpg');</v>
       </c>
     </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B41" s="1">
         <v>40</v>
       </c>
@@ -2869,7 +3005,7 @@
       <c r="G41" t="s">
         <v>199</v>
       </c>
-      <c r="H41" s="7">
+      <c r="H41" s="5">
         <v>13240</v>
       </c>
       <c r="I41" s="1">
@@ -2877,6 +3013,10 @@
       </c>
       <c r="J41" s="1">
         <v>10</v>
+      </c>
+      <c r="K41" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Mouse Redragon Storm Elite M988', 'RGB Black', '6', '7', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_20297_Mouse_Redragon_Storm_Elite_M988_RGB_Black_f25e5643-grn.jpg', '13240', '1', '10');</v>
       </c>
       <c r="L41">
         <v>3</v>
@@ -2885,11 +3025,11 @@
         <v>73</v>
       </c>
       <c r="N41" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('3','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_33878_Monitor_ASUS_24__VA24EHE-J_Full_HD_ac877e59-grn.jpg');</v>
       </c>
     </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B42" s="1">
         <v>41</v>
       </c>
@@ -2908,7 +3048,7 @@
       <c r="G42" t="s">
         <v>205</v>
       </c>
-      <c r="H42" s="7">
+      <c r="H42" s="5">
         <v>3000</v>
       </c>
       <c r="I42" s="1">
@@ -2916,6 +3056,10 @@
       </c>
       <c r="J42" s="1">
         <v>10</v>
+      </c>
+      <c r="K42" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Mouse Logitech M110S', 'Negro Blue USB', '5', '7', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_18989_Mouse_Logitech_M110S_Negro_Blue_USB_9ecef8f4-grn.jpg', '3000', '1', '10');</v>
       </c>
       <c r="L42">
         <v>3</v>
@@ -2924,11 +3068,11 @@
         <v>74</v>
       </c>
       <c r="N42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('3','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_33879_Monitor_ASUS_24__VA24EHE-J_Full_HD_e5e827ed-grn.jpg');</v>
       </c>
     </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B43" s="1">
         <v>42</v>
       </c>
@@ -2947,7 +3091,7 @@
       <c r="G43" t="s">
         <v>207</v>
       </c>
-      <c r="H43" s="7">
+      <c r="H43" s="5">
         <v>3000</v>
       </c>
       <c r="I43" s="1">
@@ -2955,6 +3099,10 @@
       </c>
       <c r="J43" s="1">
         <v>10</v>
+      </c>
+      <c r="K43" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Mouse Logitech M110S', 'Red Blue USB', '5', '7', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_24397_Mouse_Logitech_M110S_Red_520ace37-grn.jpg', '3000', '1', '10');</v>
       </c>
       <c r="L43">
         <v>3</v>
@@ -2963,11 +3111,11 @@
         <v>75</v>
       </c>
       <c r="N43" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('3','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_33881_Monitor_ASUS_24__VA24EHE-J_Full_HD_699389e6-med.jpg');</v>
       </c>
     </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B44" s="1">
         <v>43</v>
       </c>
@@ -2986,7 +3134,7 @@
       <c r="G44" t="s">
         <v>212</v>
       </c>
-      <c r="H44" s="7">
+      <c r="H44" s="5">
         <v>18600</v>
       </c>
       <c r="I44" s="1">
@@ -2994,6 +3142,10 @@
       </c>
       <c r="J44" s="1">
         <v>10</v>
+      </c>
+      <c r="K44" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Mouse Logitech G305', 'Lightspeed Wireless Blue', '5', '7', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_21243_Mouse_Logitech_G305_Lightspeed_Wireless_Blue_9c250057-grn.jpg', '18600', '1', '10');</v>
       </c>
       <c r="L44">
         <v>4</v>
@@ -3002,11 +3154,11 @@
         <v>80</v>
       </c>
       <c r="N44" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('4','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_33822_Monitor_ASUS_27__Full_HD_HDMI_VGA_VA27EHE-J_8b229ce8-grn.jpg');</v>
       </c>
     </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B45" s="1">
         <v>44</v>
       </c>
@@ -3025,7 +3177,7 @@
       <c r="G45" t="s">
         <v>221</v>
       </c>
-      <c r="H45" s="7">
+      <c r="H45" s="5">
         <v>32000</v>
       </c>
       <c r="I45" s="1">
@@ -3033,6 +3185,10 @@
       </c>
       <c r="J45" s="1">
         <v>10</v>
+      </c>
+      <c r="K45" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Auriculares Redragon Zeus', 'RGB 7.1 Surround*', '6', '8', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_36399_Auriculares_Redragon_Zeus_X_H510-RGB_7.1_Surround__a5046a9f-grn.jpg', '32000', '1', '10');</v>
       </c>
       <c r="L45">
         <v>4</v>
@@ -3041,11 +3197,11 @@
         <v>81</v>
       </c>
       <c r="N45" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('4','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_33823_Monitor_ASUS_27__Full_HD_HDMI_VGA_VA27EHE-J_45efe665-grn.jpg');</v>
       </c>
     </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B46" s="1">
         <v>45</v>
       </c>
@@ -3064,7 +3220,7 @@
       <c r="G46" t="s">
         <v>225</v>
       </c>
-      <c r="H46" s="7">
+      <c r="H46" s="5">
         <v>30000</v>
       </c>
       <c r="I46" s="1">
@@ -3072,6 +3228,10 @@
       </c>
       <c r="J46" s="1">
         <v>10</v>
+      </c>
+      <c r="K46" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Auriculares Redragon Icon H520', 'PC PS4', '6', '8', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_29699_Auriculares_Redragon_Icon_H520_PC_PS4_42412af1-grn.jpg', '30000', '1', '10');</v>
       </c>
       <c r="L46">
         <v>4</v>
@@ -3080,11 +3240,11 @@
         <v>82</v>
       </c>
       <c r="N46" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('4','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_33824_Monitor_ASUS_27__Full_HD_HDMI_VGA_VA27EHE-J_e7f15015-grn.jpg');</v>
       </c>
     </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B47" s="1">
         <v>46</v>
       </c>
@@ -3103,7 +3263,7 @@
       <c r="G47" t="s">
         <v>229</v>
       </c>
-      <c r="H47" s="7">
+      <c r="H47" s="5">
         <v>24200</v>
       </c>
       <c r="I47" s="1">
@@ -3111,6 +3271,10 @@
       </c>
       <c r="J47" s="1">
         <v>10</v>
+      </c>
+      <c r="K47" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Auriculares HP HyperX Cloud Stinger Gaming', 'Negro  PC | PS4 | Switch | XBOX', '7', '8', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_9612_Auriculares_HP_HyperX_Cloud_Stinger_Gaming_Negro__PC___PS4___Switch___XBOX_27f1808e-grn.jpg', '24200', '1', '10');</v>
       </c>
       <c r="L47">
         <v>7</v>
@@ -3119,11 +3283,11 @@
         <v>83</v>
       </c>
       <c r="N47" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('7','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_36639_Placa_de_Video_MSI_GeForce_RTX_3090_24GB_GDDR6X_VENTUS_3X_OC_58618d16-grn.jpg');</v>
       </c>
     </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B48" s="1">
         <v>47</v>
       </c>
@@ -3142,7 +3306,7 @@
       <c r="G48" t="s">
         <v>233</v>
       </c>
-      <c r="H48" s="7">
+      <c r="H48" s="5">
         <v>32000</v>
       </c>
       <c r="I48" s="1">
@@ -3150,6 +3314,10 @@
       </c>
       <c r="J48" s="1">
         <v>10</v>
+      </c>
+      <c r="K48" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Auriculares HP HyperX Cloud', 'Black Blue PS4 PS5', '7', '8', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_35919_Auriculares_HP_HyperX_Cloud_Black_Blue_PS4_PS5_bdb54c92-grn.jpg', '32000', '1', '10');</v>
       </c>
       <c r="L48">
         <v>7</v>
@@ -3158,11 +3326,11 @@
         <v>84</v>
       </c>
       <c r="N48" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('7','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_21085_Placa_de_Video_MSI_GeForce_RTX_3090_24GB_GDDR6X_VENTUS_3X_OC_8ab3b437-grn.jpg');</v>
       </c>
     </row>
-    <row r="49" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B49" s="1">
         <v>48</v>
       </c>
@@ -3181,7 +3349,7 @@
       <c r="G49" t="s">
         <v>237</v>
       </c>
-      <c r="H49" s="7">
+      <c r="H49" s="5">
         <v>11000</v>
       </c>
       <c r="I49" s="1">
@@ -3189,6 +3357,10 @@
       </c>
       <c r="J49" s="1">
         <v>10</v>
+      </c>
+      <c r="K49" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Auriculares Genius GX', ' Gaming HS-G710V', '8', '8', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_31170_Auriculares_Genius_GX_Gaming_HS-G710V_e7832ba5-grn.jpg', '11000', '1', '10');</v>
       </c>
       <c r="L49">
         <v>7</v>
@@ -3197,11 +3369,11 @@
         <v>85</v>
       </c>
       <c r="N49" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('7','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_21087_Placa_de_Video_MSI_GeForce_RTX_3090_24GB_GDDR6X_VENTUS_3X_OC_4842e14d-grn.jpg');</v>
       </c>
     </row>
-    <row r="50" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B50" s="1">
         <v>49</v>
       </c>
@@ -3220,7 +3392,7 @@
       <c r="G50" t="s">
         <v>217</v>
       </c>
-      <c r="H50" s="7">
+      <c r="H50" s="5">
         <v>22000</v>
       </c>
       <c r="I50" s="1">
@@ -3228,6 +3400,10 @@
       </c>
       <c r="J50" s="1">
         <v>10</v>
+      </c>
+      <c r="K50" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Auriculares Logitech G335', 'White', '5', '8', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_27936_Auriculares_Logitech_G335_White_32282a6d-grn.jpg', '22000', '1', '10');</v>
       </c>
       <c r="L50">
         <v>8</v>
@@ -3236,11 +3412,11 @@
         <v>90</v>
       </c>
       <c r="N50" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('8','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_36550_Placa_de_Video_ASUS_Phoenix_GeForce_GTX_1630_4GB_GDDR6_b0a0edd2-grn.jpg');</v>
       </c>
     </row>
-    <row r="51" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B51" s="1">
         <v>50</v>
       </c>
@@ -3256,7 +3432,7 @@
       <c r="G51" t="s">
         <v>240</v>
       </c>
-      <c r="H51" s="7">
+      <c r="H51" s="5">
         <v>55000</v>
       </c>
       <c r="I51" s="1">
@@ -3264,6 +3440,10 @@
       </c>
       <c r="J51" s="1">
         <v>10</v>
+      </c>
+      <c r="K51" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Mother MSI A520M-A PRO AM4', '', '2', '9', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_21848_Mother_MSI_A520M-A_PRO_AM4_29d05f8c-grn.jpg', '55000', '1', '10');</v>
       </c>
       <c r="L51">
         <v>8</v>
@@ -3272,11 +3452,11 @@
         <v>91</v>
       </c>
       <c r="N51" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('8','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_36551_Placa_de_Video_ASUS_Phoenix_GeForce_GTX_1630_4GB_GDDR6_0aa6ea72-grn.jpg');</v>
       </c>
     </row>
-    <row r="52" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B52" s="1">
         <v>51</v>
       </c>
@@ -3292,7 +3472,7 @@
       <c r="G52" t="s">
         <v>243</v>
       </c>
-      <c r="H52" s="7">
+      <c r="H52" s="5">
         <v>57750</v>
       </c>
       <c r="I52" s="1">
@@ -3300,6 +3480,10 @@
       </c>
       <c r="J52" s="1">
         <v>10</v>
+      </c>
+      <c r="K52" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Mother ASUS PRIME A520M-K AM4', '', '1', '9', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_20551_Mother_ASUS_PRIME_A520M-K_AM4_f5d89e00-grn.jpg', '57750', '1', '10');</v>
       </c>
       <c r="L52">
         <v>9</v>
@@ -3308,11 +3492,11 @@
         <v>94</v>
       </c>
       <c r="N52" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('9','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_35211_Placa_de_Video_ASUS_GeForce_GTX_1660_SUPER_6GB_GDDR6_OC_TUF_91e6cd72-grn.jpg');</v>
       </c>
     </row>
-    <row r="53" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B53" s="1">
         <v>52</v>
       </c>
@@ -3328,7 +3512,7 @@
       <c r="G53" t="s">
         <v>246</v>
       </c>
-      <c r="H53" s="7">
+      <c r="H53" s="5">
         <v>71000</v>
       </c>
       <c r="I53" s="1">
@@ -3336,6 +3520,10 @@
       </c>
       <c r="J53" s="1">
         <v>10</v>
+      </c>
+      <c r="K53" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Mother MSI B450 Gaming Plus Max AM4', '', '2', '9', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_25784_Mother_MSI_B450_Gaming_Plus_Max_AM4_5dd0dc29-grn.jpg', '71000', '1', '10');</v>
       </c>
       <c r="L53">
         <v>9</v>
@@ -3344,11 +3532,11 @@
         <v>95</v>
       </c>
       <c r="N53" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('9','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_17243_Placa_de_Video_ASUS_GeForce_GTX_1660_SUPER_6GB_GDDR6_OC_TUF_9b71c1cd-grn.jpg');</v>
       </c>
     </row>
-    <row r="54" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B54" s="1">
         <v>53</v>
       </c>
@@ -3364,7 +3552,7 @@
       <c r="G54" t="s">
         <v>249</v>
       </c>
-      <c r="H54" s="7">
+      <c r="H54" s="5">
         <v>98000</v>
       </c>
       <c r="I54" s="1">
@@ -3372,6 +3560,10 @@
       </c>
       <c r="J54" s="1">
         <v>10</v>
+      </c>
+      <c r="K54" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Mother MSI X570-A PRO AM4', '', '2', '9', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_15692_Mother_MSI_X570-A_PRO_AM4_bbf981bd-grn.jpg', '98000', '1', '10');</v>
       </c>
       <c r="L54">
         <v>9</v>
@@ -3380,11 +3572,11 @@
         <v>96</v>
       </c>
       <c r="N54" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('9','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_17244_Placa_de_Video_ASUS_GeForce_GTX_1660_SUPER_6GB_GDDR6_OC_TUF_04cc5a64-grn.jpg');</v>
       </c>
     </row>
-    <row r="55" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B55" s="1">
         <v>54</v>
       </c>
@@ -3400,7 +3592,7 @@
       <c r="G55" t="s">
         <v>252</v>
       </c>
-      <c r="H55" s="7">
+      <c r="H55" s="5">
         <v>53500</v>
       </c>
       <c r="I55" s="1">
@@ -3408,6 +3600,10 @@
       </c>
       <c r="J55" s="1">
         <v>10</v>
+      </c>
+      <c r="K55" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Mother ASUS PRIME H610M-E D4 S1700', '', '1', '9', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_30440_Mother_ASUS_PRIME_H610M-E_D4_S1700_3402c168-grn.jpg', '53500', '1', '10');</v>
       </c>
       <c r="L55">
         <v>10</v>
@@ -3416,11 +3612,11 @@
         <v>99</v>
       </c>
       <c r="N55" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('10','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_27548_Placa_de_Video_ASUS_GeForce_GTX_1650_4GB_GDDR6_TUF_GAMING_71e82ff4-grn.jpg');</v>
       </c>
     </row>
-    <row r="56" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B56" s="1">
         <v>55</v>
       </c>
@@ -3436,7 +3632,7 @@
       <c r="G56" t="s">
         <v>255</v>
       </c>
-      <c r="H56" s="7">
+      <c r="H56" s="5">
         <v>53000</v>
       </c>
       <c r="I56" s="1">
@@ -3444,6 +3640,10 @@
       </c>
       <c r="J56" s="1">
         <v>10</v>
+      </c>
+      <c r="K56" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Mother Asrock H610M-HVS LGA 1700', '', '11', '9', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_34006_Mother_Asrock_H610M-HVS_LGA_1700_486791bd-grn.jpg', '53000', '1', '10');</v>
       </c>
       <c r="L56">
         <v>10</v>
@@ -3452,11 +3652,11 @@
         <v>100</v>
       </c>
       <c r="N56" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('10','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_16562_Placa_de_Video_ASUS_GeForce_GTX_1650_4GB_GDDR6_TUF_GAMING_25c172c8-grn.jpg');</v>
       </c>
     </row>
-    <row r="57" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B57" s="1">
         <v>56</v>
       </c>
@@ -3472,7 +3672,7 @@
       <c r="G57" t="s">
         <v>257</v>
       </c>
-      <c r="H57" s="7">
+      <c r="H57" s="5">
         <v>52000</v>
       </c>
       <c r="I57" s="1">
@@ -3480,6 +3680,10 @@
       </c>
       <c r="J57" s="1">
         <v>10</v>
+      </c>
+      <c r="K57" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Mother Asrock A520M-HDV AM4', '', '11', '9', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_24392_Mother_Asrock_A520M-HDV_AM4_5c7ae4d7-grn.jpg', '52000', '1', '10');</v>
       </c>
       <c r="L57">
         <v>11</v>
@@ -3488,11 +3692,11 @@
         <v>105</v>
       </c>
       <c r="N57" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('11','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_19289_Placa_de_Video_Asrock_Radeon_RX_550_2GB_GDDR5_Phantom_Gaming_99528ce8-grn.jpg');</v>
       </c>
     </row>
-    <row r="58" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B58" s="1">
         <v>57</v>
       </c>
@@ -3511,7 +3715,7 @@
       <c r="G58" t="s">
         <v>262</v>
       </c>
-      <c r="H58" s="7">
+      <c r="H58" s="5">
         <v>94000</v>
       </c>
       <c r="I58" s="1">
@@ -3519,6 +3723,10 @@
       </c>
       <c r="J58" s="1">
         <v>10</v>
+      </c>
+      <c r="K58" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Procesador AMD RYZEN 5 3600', '4.2GHz Turbo AM4 Wraith Stealth Cooler', '3', '10', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_16749_Procesador_AMD_RYZEN_5_3600_4.2GHz_Turbo_AM4_Wraith_Stealth_Cooler_f8ab4915-grn.jpg', '94000', '1', '10');</v>
       </c>
       <c r="L58">
         <v>11</v>
@@ -3527,11 +3735,11 @@
         <v>106</v>
       </c>
       <c r="N58" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('11','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_19290_Placa_de_Video_Asrock_Radeon_RX_550_2GB_GDDR5_Phantom_Gaming_1e8baa4a-grn.jpg');</v>
       </c>
     </row>
-    <row r="59" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B59" s="1">
         <v>58</v>
       </c>
@@ -3550,7 +3758,7 @@
       <c r="G59" t="s">
         <v>266</v>
       </c>
-      <c r="H59" s="7">
+      <c r="H59" s="5">
         <v>100000</v>
       </c>
       <c r="I59" s="1">
@@ -3558,6 +3766,10 @@
       </c>
       <c r="J59" s="1">
         <v>10</v>
+      </c>
+      <c r="K59" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Procesador AMD Ryzen 5 5500', '4.2GHz Turbo + Wraith Stealth Cooler', '3', '10', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_31696_Procesador_AMD_Ryzen_5_5500_4.2GHz_Turbo___Wraith_Stealth_Cooler_ca9fc7de-grn.jpg', '100000', '1', '10');</v>
       </c>
       <c r="L59">
         <v>12</v>
@@ -3566,11 +3778,11 @@
         <v>109</v>
       </c>
       <c r="N59" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('12','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_29154_Placa_de_Video_Asrock_Radeon_RX_6800_XT_16GB_GDDR6_Phantom_Gaming_D_OC_b76349fe-grn.jpg');</v>
       </c>
     </row>
-    <row r="60" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B60" s="1">
         <v>59</v>
       </c>
@@ -3589,7 +3801,7 @@
       <c r="G60" t="s">
         <v>269</v>
       </c>
-      <c r="H60" s="7">
+      <c r="H60" s="5">
         <v>250000</v>
       </c>
       <c r="I60" s="1">
@@ -3597,6 +3809,10 @@
       </c>
       <c r="J60" s="1">
         <v>10</v>
+      </c>
+      <c r="K60" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Procesador AMD Ryzen 9 5950X', '4.9GHz Turbo AM4 - No incluye Cooler', '3', '10', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_22302_Procesador_AMD_Ryzen_9_5950X_4.9GHz_Turbo_AM4_-_No_incluye_Cooler_9d34d3b3-grn.jpg', '250000', '1', '10');</v>
       </c>
       <c r="L60">
         <v>12</v>
@@ -3605,11 +3821,11 @@
         <v>110</v>
       </c>
       <c r="N60" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('12','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_29155_Placa_de_Video_Asrock_Radeon_RX_6800_XT_16GB_GDDR6_Phantom_Gaming_D_OC_f28765e9-grn.jpg');</v>
       </c>
     </row>
-    <row r="61" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B61" s="1">
         <v>60</v>
       </c>
@@ -3628,7 +3844,7 @@
       <c r="G61" t="s">
         <v>272</v>
       </c>
-      <c r="H61" s="7">
+      <c r="H61" s="5">
         <v>19000</v>
       </c>
       <c r="I61" s="1">
@@ -3636,6 +3852,10 @@
       </c>
       <c r="J61" s="1">
         <v>10</v>
+      </c>
+      <c r="K61" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Procesador Intel Pentium G4560', '3.5GHz Socket 1151 Kaby Lake OEM Sin Cooler', '4', '10', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_13151_Procesador_Intel_Pentium_G4560_3.5GHz_Socket_1151_Kaby_Lake_OEM_Sin_Cooler_58161f82-grn.jpg', '19000', '1', '10');</v>
       </c>
       <c r="L61">
         <v>12</v>
@@ -3644,11 +3864,11 @@
         <v>111</v>
       </c>
       <c r="N61" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('12','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_29157_Placa_de_Video_Asrock_Radeon_RX_6800_XT_16GB_GDDR6_Phantom_Gaming_D_OC_b3f0fc37-grn.jpg');</v>
       </c>
     </row>
-    <row r="62" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B62" s="1">
         <v>61</v>
       </c>
@@ -3667,7 +3887,7 @@
       <c r="G62" t="s">
         <v>273</v>
       </c>
-      <c r="H62" s="7">
+      <c r="H62" s="5">
         <v>191500</v>
       </c>
       <c r="I62" s="1">
@@ -3675,6 +3895,10 @@
       </c>
       <c r="J62" s="1">
         <v>10</v>
+      </c>
+      <c r="K62" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Procesador Intel Core i7 10700', '4.8GHz Turbo Socket 1200 Comet Lake', '4', '10', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_19228_Procesador_Intel_Core_i7_10700_4.8GHz_Turbo_Socket_1200_Comet_Lake_e3d7d847-grn.jpg', '191500', '1', '10');</v>
       </c>
       <c r="L62">
         <v>13</v>
@@ -3683,11 +3907,11 @@
         <v>114</v>
       </c>
       <c r="N62" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('13','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_32107_Disco_Solido_SSD_M.2_WD_500GB_Blue_SN570_3500MB_s_NVMe_PCI-E_Gen3_x4_TLC_3135e1e9-grn.jpg');</v>
       </c>
     </row>
-    <row r="63" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B63" s="1">
         <v>62</v>
       </c>
@@ -3706,7 +3930,7 @@
       <c r="G63" t="s">
         <v>278</v>
       </c>
-      <c r="H63" s="7">
+      <c r="H63" s="5">
         <v>140000</v>
       </c>
       <c r="I63" s="1">
@@ -3714,6 +3938,10 @@
       </c>
       <c r="J63" s="1">
         <v>10</v>
+      </c>
+      <c r="K63" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ARTICULOS VALUES ( 'Procesador Intel Core i5 11600KF', '4.9GHz Turbo Socket 1200 Rocket Lake', '4', '10', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_25668_Procesador_Intel_Core_i5_11600KF_4.9GHz_Turbo_Socket_1200_Rocket_Lake_7f61810f-grn.jpg', '140000', '1', '10');</v>
       </c>
       <c r="L63">
         <v>13</v>
@@ -3722,7 +3950,7 @@
         <v>115</v>
       </c>
       <c r="N63" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('13','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_32108_Disco_Solido_SSD_M.2_WD_500GB_Blue_SN570_3500MB_s_NVMe_PCI-E_Gen3_x4_TLC_9a9da7d5-grn.jpg');</v>
       </c>
     </row>
@@ -3734,7 +3962,7 @@
         <v>118</v>
       </c>
       <c r="N64" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('14','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_28600_Disco_Solido_SSD_M.2_WD_500GB_Black_SN750_SE_3600MB_s_PCI-E_X4_NVMe_GEN4_b815bec0-grn.jpg');</v>
       </c>
     </row>
@@ -3746,7 +3974,7 @@
         <v>119</v>
       </c>
       <c r="N65" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('14','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_28602_Disco_Solido_SSD_M.2_WD_500GB_Black_SN750_SE_3600MB_s_PCI-E_X4_NVMe_GEN4_654966d5-grn.jpg');</v>
       </c>
     </row>
@@ -3758,7 +3986,7 @@
         <v>122</v>
       </c>
       <c r="N66" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('15','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_33159_Disco_Solido_SSD_M.2_WD_500GB_WD_Black_SN770_5000MB_s_NVMe_PCI-E_x4_Gen_4_7a4a307b-grn.jpg');</v>
       </c>
     </row>
@@ -3770,7 +3998,7 @@
         <v>123</v>
       </c>
       <c r="N67" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('15','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_33160_Disco_Solido_SSD_M.2_WD_500GB_WD_Black_SN770_5000MB_s_NVMe_PCI-E_x4_Gen_4_2aff08dd-grn.jpg');</v>
       </c>
     </row>
@@ -3782,7 +4010,7 @@
         <v>126</v>
       </c>
       <c r="N68" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('16','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_35589_Disco_Solido_SSD_M.2_WD_1TB_WD_Black_SN770_5150MB_s_NVMe_PCI-E_x4_Gen_4_7a4a307b-grn.jpg');</v>
       </c>
     </row>
@@ -3794,7 +4022,7 @@
         <v>127</v>
       </c>
       <c r="N69" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('16','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_33622_Disco_Solido_SSD_M.2_WD_1TB_WD_Black_SN770_5150MB_s_NVMe_PCI-E_x4_Gen_4_60cef2e6-grn.jpg');</v>
       </c>
     </row>
@@ -3806,7 +4034,7 @@
         <v>130</v>
       </c>
       <c r="N70" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('17','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_29777_Disco_Solido_SSD_Adata_240GB_SU650SS_520MB_s__8b455937-grn.jpg');</v>
       </c>
     </row>
@@ -3818,7 +4046,7 @@
         <v>131</v>
       </c>
       <c r="N71" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('17','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_29778_Disco_Solido_SSD_Adata_240GB_SU650SS_520MB_s__c1c34d0c-grn.jpg');</v>
       </c>
     </row>
@@ -3830,7 +4058,7 @@
         <v>134</v>
       </c>
       <c r="N72" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('18','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_9018_Disco_R__gido_WD_1TB_BLUE_64MB_SATA_6.0GB_s__ca74d162-grn.jpg');</v>
       </c>
     </row>
@@ -3842,7 +4070,7 @@
         <v>135</v>
       </c>
       <c r="N73" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('18','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_1196_Disco_R__gido_WD_1TB_BLUE_64MB_SATA_6.0GB_s__1545a4f9-grn.jpg');</v>
       </c>
     </row>
@@ -3854,7 +4082,7 @@
         <v>138</v>
       </c>
       <c r="N74" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('19','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_21014_Disco_Rigido_WD_2TB_BLUE_256MB_SATA_6.0GB_s_44f766ac-grn.jpg');</v>
       </c>
     </row>
@@ -3866,7 +4094,7 @@
         <v>139</v>
       </c>
       <c r="N75" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('20','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_21015_Disco_Rigido_WD_2TB_BLUE_256MB_SATA_6.0GB_s_d1e138ed-grn.jpg');</v>
       </c>
     </row>
@@ -3878,7 +4106,7 @@
         <v>141</v>
       </c>
       <c r="N76" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('21','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_35996_Disco_Rigido_WD_2TB_BLUE_256MB_SATA_6.0GB_s_7200RPM_dc36f8f5-grn.jpg');</v>
       </c>
     </row>
@@ -3890,7 +4118,7 @@
         <v>144</v>
       </c>
       <c r="N77" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('22','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_26480_Disco_Rigido_WD_12TB_Red_Pro_7.2K_RPM_256MB_c66a3fa3-grn.jpg');</v>
       </c>
     </row>
@@ -3902,7 +4130,7 @@
         <v>147</v>
       </c>
       <c r="N78" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('23','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_26484_Disco_Rigido_WD_12TB_Gold_7.2K_RPM_256MB_856fe552-grn.jpg');</v>
       </c>
     </row>
@@ -3914,7 +4142,7 @@
         <v>152</v>
       </c>
       <c r="N79" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('24','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_13221_Memoria_Adata_DDR4_4GB_2666MHz_Value__aa6df289-grn.jpg');</v>
       </c>
     </row>
@@ -3926,7 +4154,7 @@
         <v>155</v>
       </c>
       <c r="N80" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('25','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_16184_Memoria_Adata_DDR4_8GB_2666MHz_Value_Sodimm_Notebook_38c2e2af-grn.jpg');</v>
       </c>
     </row>
@@ -3938,7 +4166,7 @@
         <v>158</v>
       </c>
       <c r="N81" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('26','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_18814_Memoria_Adata_DDR4_8GB_3200MHz_Premier_c6036c27-grn.jpg');</v>
       </c>
     </row>
@@ -3950,7 +4178,7 @@
         <v>159</v>
       </c>
       <c r="N82" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('27','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_25890_Memoria_Adata_DDR4_16GB_3200MHz_CL16_XPG_GAMMIX_D20_Black_6b1582d3-grn.jpg');</v>
       </c>
     </row>
@@ -3962,7 +4190,7 @@
         <v>163</v>
       </c>
       <c r="N83" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('28','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_28924_Memoria_Adata_DDR4_8GB_3200MHz_XPG_Spectrix_D60G_RGB_Titanium_88f51e0f-grn.jpg');</v>
       </c>
     </row>
@@ -3974,7 +4202,7 @@
         <v>165</v>
       </c>
       <c r="N84" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('29','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_28926_Memoria_Adata_DDR4_8GB_3200MHz_XPG_Spectrix_D50_RGB_Titanium_446ebe28-grn.jpg');</v>
       </c>
     </row>
@@ -3986,7 +4214,7 @@
         <v>168</v>
       </c>
       <c r="N85" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('30','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_29885_Memoria_Adata_DDR4__2x8GB__16GB_5000MHz_XPG_Spectrix_D50_Xtreme_RGB_CL19_18133a6d-grn.jpg');</v>
       </c>
     </row>
@@ -3998,7 +4226,7 @@
         <v>173</v>
       </c>
       <c r="N86" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('31','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_33275_Teclado_Mecanico_Logitech_PRO_TKL_LOL_2_Switch_Brown_30e10b48-grn.jpg');</v>
       </c>
     </row>
@@ -4010,7 +4238,7 @@
         <v>176</v>
       </c>
       <c r="N87" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('32','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_19865_Teclado_Mecanico_Logitech_G513_Carbon_RGB_Switch_GX_Brown_Espa__ol_9ccf7c47-grn.jpg');</v>
       </c>
     </row>
@@ -4022,7 +4250,7 @@
         <v>179</v>
       </c>
       <c r="N88" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('33','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_33269_Teclado_Mecanico_Logitech_POP_Blast_Yellow_Wireless_725996a0-grn.jpg');</v>
       </c>
     </row>
@@ -4034,7 +4262,7 @@
         <v>182</v>
       </c>
       <c r="N89" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('34','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_36665_Teclado_Mecanico_Logitech_POP_Coral_Rose_Wireless_065ab138-grn.jpg');</v>
       </c>
     </row>
@@ -4046,7 +4274,7 @@
         <v>185</v>
       </c>
       <c r="N90" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('35','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_16207_Teclado_Logitech_G815_Mechanical_RGB_Lightsync_5ab9b8b1-grn.jpg');</v>
       </c>
     </row>
@@ -4058,7 +4286,7 @@
         <v>188</v>
       </c>
       <c r="N91" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('36','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_19373_Teclado_Mecanico_Logitech_G915_TKL_RGB_Lightspeed_Inalambrico_065f0cec-grn.jpg');</v>
       </c>
     </row>
@@ -4070,7 +4298,7 @@
         <v>193</v>
       </c>
       <c r="N92" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('38','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_28612_Mouse_Redragon_Centrophorus_M601_RGB_e00743a5-grn.jpg');</v>
       </c>
     </row>
@@ -4082,7 +4310,7 @@
         <v>194</v>
       </c>
       <c r="N93" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('38','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_28614_Mouse_Redragon_Centrophorus_M601_RGB_9e2363c4-grn.jpg');</v>
       </c>
     </row>
@@ -4094,7 +4322,7 @@
         <v>197</v>
       </c>
       <c r="N94" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('39','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_8760_Mouse_Redragon_Mirage_M690_2.5GHz_Wireless_1739dc55-grn.jpg');</v>
       </c>
     </row>
@@ -4106,7 +4334,7 @@
         <v>198</v>
       </c>
       <c r="N95" t="str">
-        <f t="shared" ref="N95:N137" si="3">CONCATENATE("INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('", L95, "','", TEXT(M95,"0"), "');")</f>
+        <f t="shared" ref="N95:N137" si="4">CONCATENATE("INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('", L95, "','", TEXT(M95,"0"), "');")</f>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('39','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_8759_Mouse_Redragon_Mirage_M690_2.5GHz_Wireless_13e59d69-grn.jpg');</v>
       </c>
     </row>
@@ -4118,7 +4346,7 @@
         <v>199</v>
       </c>
       <c r="N96" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('40','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_20297_Mouse_Redragon_Storm_Elite_M988_RGB_Black_f25e5643-grn.jpg');</v>
       </c>
     </row>
@@ -4130,7 +4358,7 @@
         <v>200</v>
       </c>
       <c r="N97" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('40','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_20299_Mouse_Redragon_Storm_Elite_M988_RGB_Black_da0b8b96-grn.jpg');</v>
       </c>
     </row>
@@ -4142,7 +4370,7 @@
         <v>205</v>
       </c>
       <c r="N98" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('41','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_18989_Mouse_Logitech_M110S_Negro_Blue_USB_9ecef8f4-grn.jpg');</v>
       </c>
     </row>
@@ -4154,7 +4382,7 @@
         <v>206</v>
       </c>
       <c r="N99" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('41','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_18992_Mouse_Logitech_M110S_Negro_Blue_USB_f0eff56d-med.jpg');</v>
       </c>
     </row>
@@ -4166,7 +4394,7 @@
         <v>207</v>
       </c>
       <c r="N100" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('42','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_24397_Mouse_Logitech_M110S_Red_520ace37-grn.jpg');</v>
       </c>
     </row>
@@ -4178,7 +4406,7 @@
         <v>208</v>
       </c>
       <c r="N101" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('42','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_24400_Mouse_Logitech_M110S_Red_572df13e-grn.jpg');</v>
       </c>
     </row>
@@ -4190,7 +4418,7 @@
         <v>212</v>
       </c>
       <c r="N102" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('43','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_21243_Mouse_Logitech_G305_Lightspeed_Wireless_Blue_9c250057-grn.jpg');</v>
       </c>
     </row>
@@ -4202,7 +4430,7 @@
         <v>213</v>
       </c>
       <c r="N103" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('43','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_21245_Mouse_Logitech_G305_Lightspeed_Wireless_Blue_44244ac2-grn.jpg');</v>
       </c>
     </row>
@@ -4214,7 +4442,7 @@
         <v>214</v>
       </c>
       <c r="N104" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('43','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_21248_Mouse_Logitech_G305_Lightspeed_Wireless_Blue_d27a8d95-grn.jpg');</v>
       </c>
     </row>
@@ -4226,7 +4454,7 @@
         <v>221</v>
       </c>
       <c r="N105" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('44','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_36399_Auriculares_Redragon_Zeus_X_H510-RGB_7.1_Surround__a5046a9f-grn.jpg');</v>
       </c>
     </row>
@@ -4238,7 +4466,7 @@
         <v>222</v>
       </c>
       <c r="N106" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('44','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_36400_Auriculares_Redragon_Zeus_X_H510-RGB_7.1_Surround__a6d2f307-grn.jpg');</v>
       </c>
     </row>
@@ -4250,7 +4478,7 @@
         <v>225</v>
       </c>
       <c r="N107" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('45','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_29699_Auriculares_Redragon_Icon_H520_PC_PS4_42412af1-grn.jpg');</v>
       </c>
     </row>
@@ -4262,7 +4490,7 @@
         <v>226</v>
       </c>
       <c r="N108" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('45','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_29700_Auriculares_Redragon_Icon_H520_PC_PS4_99b94941-grn.jpg');</v>
       </c>
     </row>
@@ -4274,7 +4502,7 @@
         <v>229</v>
       </c>
       <c r="N109" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('46','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_9612_Auriculares_HP_HyperX_Cloud_Stinger_Gaming_Negro__PC___PS4___Switch___XBOX_27f1808e-grn.jpg');</v>
       </c>
     </row>
@@ -4286,7 +4514,7 @@
         <v>230</v>
       </c>
       <c r="N110" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('46','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_9613_Auriculares_HP_HyperX_Cloud_Stinger_Gaming_Negro__PC___PS4___Switch___XBOX_c8b462ee-grn.jpg');</v>
       </c>
     </row>
@@ -4298,7 +4526,7 @@
         <v>233</v>
       </c>
       <c r="N111" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('47','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_35919_Auriculares_HP_HyperX_Cloud_Black_Blue_PS4_PS5_bdb54c92-grn.jpg');</v>
       </c>
     </row>
@@ -4310,7 +4538,7 @@
         <v>234</v>
       </c>
       <c r="N112" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('47','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_35920_Auriculares_HP_HyperX_Cloud_Black_Blue_PS4_PS5_e80b9f85-grn.jpg');</v>
       </c>
     </row>
@@ -4322,7 +4550,7 @@
         <v>238</v>
       </c>
       <c r="N113" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('48','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_31171_Auriculares_Genius_GX_Gaming_HS-G710V_91b68c27-grn.jpg');</v>
       </c>
     </row>
@@ -4334,7 +4562,7 @@
         <v>237</v>
       </c>
       <c r="N114" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('48','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_31170_Auriculares_Genius_GX_Gaming_HS-G710V_e7832ba5-grn.jpg');</v>
       </c>
     </row>
@@ -4346,7 +4574,7 @@
         <v>217</v>
       </c>
       <c r="N115" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('49','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_27936_Auriculares_Logitech_G335_White_32282a6d-grn.jpg');</v>
       </c>
     </row>
@@ -4358,7 +4586,7 @@
         <v>218</v>
       </c>
       <c r="N116" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('49','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_27937_Auriculares_Logitech_G335_White_5d46d2e5-grn.jpg');</v>
       </c>
     </row>
@@ -4370,7 +4598,7 @@
         <v>240</v>
       </c>
       <c r="N117" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('50','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_21848_Mother_MSI_A520M-A_PRO_AM4_29d05f8c-grn.jpg');</v>
       </c>
     </row>
@@ -4382,7 +4610,7 @@
         <v>241</v>
       </c>
       <c r="N118" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('50','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_21849_Mother_MSI_A520M-A_PRO_AM4_8baafa01-grn.jpg');</v>
       </c>
     </row>
@@ -4394,7 +4622,7 @@
         <v>243</v>
       </c>
       <c r="N119" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('51','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_20551_Mother_ASUS_PRIME_A520M-K_AM4_f5d89e00-grn.jpg');</v>
       </c>
     </row>
@@ -4406,7 +4634,7 @@
         <v>244</v>
       </c>
       <c r="N120" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('51','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_20553_Mother_ASUS_PRIME_A520M-K_AM4_9216f824-grn.jpg');</v>
       </c>
     </row>
@@ -4418,7 +4646,7 @@
         <v>246</v>
       </c>
       <c r="N121" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('52','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_25784_Mother_MSI_B450_Gaming_Plus_Max_AM4_5dd0dc29-grn.jpg');</v>
       </c>
     </row>
@@ -4430,7 +4658,7 @@
         <v>247</v>
       </c>
       <c r="N122" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('52','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_25785_Mother_MSI_B450_Gaming_Plus_Max_AM4_d5692b77-grn.jpg');</v>
       </c>
     </row>
@@ -4442,7 +4670,7 @@
         <v>249</v>
       </c>
       <c r="N123" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('53','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_15692_Mother_MSI_X570-A_PRO_AM4_bbf981bd-grn.jpg');</v>
       </c>
     </row>
@@ -4454,7 +4682,7 @@
         <v>250</v>
       </c>
       <c r="N124" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('53','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_15693_Mother_MSI_X570-A_PRO_AM4_b29443fe-grn.jpg');</v>
       </c>
     </row>
@@ -4466,7 +4694,7 @@
         <v>252</v>
       </c>
       <c r="N125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('54','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_30440_Mother_ASUS_PRIME_H610M-E_D4_S1700_3402c168-grn.jpg');</v>
       </c>
     </row>
@@ -4478,7 +4706,7 @@
         <v>253</v>
       </c>
       <c r="N126" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('54','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_30441_Mother_ASUS_PRIME_H610M-E_D4_S1700_b1b07b46-grn.jpg');</v>
       </c>
     </row>
@@ -4490,7 +4718,7 @@
         <v>255</v>
       </c>
       <c r="N127" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('55','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_34006_Mother_Asrock_H610M-HVS_LGA_1700_486791bd-grn.jpg');</v>
       </c>
     </row>
@@ -4502,7 +4730,7 @@
         <v>256</v>
       </c>
       <c r="N128" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('55','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_34007_Mother_Asrock_H610M-HVS_LGA_1700_7eedfce1-grn.jpg');</v>
       </c>
     </row>
@@ -4514,7 +4742,7 @@
         <v>257</v>
       </c>
       <c r="N129" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('56','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_24392_Mother_Asrock_A520M-HDV_AM4_5c7ae4d7-grn.jpg');</v>
       </c>
     </row>
@@ -4526,7 +4754,7 @@
         <v>258</v>
       </c>
       <c r="N130" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('56','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_24393_Mother_Asrock_A520M-HDV_AM4_affcd72d-grn.jpg');</v>
       </c>
     </row>
@@ -4538,7 +4766,7 @@
         <v>262</v>
       </c>
       <c r="N131" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('57','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_16749_Procesador_AMD_RYZEN_5_3600_4.2GHz_Turbo_AM4_Wraith_Stealth_Cooler_f8ab4915-grn.jpg');</v>
       </c>
     </row>
@@ -4550,7 +4778,7 @@
         <v>263</v>
       </c>
       <c r="N132" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('57','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_14074_Procesador_AMD_RYZEN_5_3600_4.2GHz_Turbo_AM4_Wraith_Stealth_Cooler_14f3a44e-grn.jpg');</v>
       </c>
     </row>
@@ -4562,7 +4790,7 @@
         <v>266</v>
       </c>
       <c r="N133" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('58','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_31696_Procesador_AMD_Ryzen_5_5500_4.2GHz_Turbo___Wraith_Stealth_Cooler_ca9fc7de-grn.jpg');</v>
       </c>
     </row>
@@ -4574,7 +4802,7 @@
         <v>269</v>
       </c>
       <c r="N134" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('59','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_22302_Procesador_AMD_Ryzen_9_5950X_4.9GHz_Turbo_AM4_-_No_incluye_Cooler_9d34d3b3-grn.jpg');</v>
       </c>
     </row>
@@ -4586,7 +4814,7 @@
         <v>272</v>
       </c>
       <c r="N135" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('60','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_13151_Procesador_Intel_Pentium_G4560_3.5GHz_Socket_1151_Kaby_Lake_OEM_Sin_Cooler_58161f82-grn.jpg');</v>
       </c>
     </row>
@@ -4598,7 +4826,7 @@
         <v>273</v>
       </c>
       <c r="N136" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('61','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_19228_Procesador_Intel_Core_i7_10700_4.8GHz_Turbo_Socket_1200_Comet_Lake_e3d7d847-grn.jpg');</v>
       </c>
     </row>
@@ -4610,7 +4838,7 @@
         <v>278</v>
       </c>
       <c r="N137" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('62','https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_25668_Procesador_Intel_Core_i5_11600KF_4.9GHz_Turbo_Socket_1200_Rocket_Lake_7f61810f-grn.jpg');</v>
       </c>
     </row>

</xml_diff>

<commit_message>
agregador de filtros, mejoras visuales y funcionalidades
</commit_message>
<xml_diff>
--- a/Carga de datos.xlsx
+++ b/Carga de datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manu\Desktop\TrabajoPracticoProgra\TPFinal-e19-Amarilla-Casulo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4BBAFF4-7E83-464D-98F6-89A50385E04F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72342198-0B16-4014-BB9E-C684AC18C10E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1240,8 +1240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" topLeftCell="B38" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K68" sqref="K68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1252,7 +1252,7 @@
     <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.7109375" customWidth="1"/>
     <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" customWidth="1"/>
+    <col min="11" max="11" width="72.85546875" customWidth="1"/>
     <col min="13" max="13" width="40" customWidth="1"/>
     <col min="14" max="14" width="22.42578125" customWidth="1"/>
     <col min="16" max="16" width="26.5703125" customWidth="1"/>
@@ -1324,8 +1324,8 @@
         <v>10</v>
       </c>
       <c r="K2" s="6" t="str">
-        <f>CONCATENATE("INSERT INTO ARTICULOS VALUES ( '",C2, "', '", D2, "', '", E2, "', '", F2, "', '", G2, "', '", H2, "', '", I2, "', '", J2, "');")</f>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Monitor ASUS 21.5"', 'VP228HE-J Full HD 1ms HDMI VGA', '1', '1', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_27034_Monitor_ASUS_21.5__VP228HE-J_Full_HD_1ms_HDMI_VGA_a797ab9e-grn.jpg', '58650', '1', '10');</v>
+        <f>CONCATENATE("INSERT INTO ARTICULOS VALUES ('",B2, "','",C2, "', '", D2, "', '", E2, "', '", F2, "', '", G2, "', '", H2, "', '", I2, "', '", J2, "');")</f>
+        <v>INSERT INTO ARTICULOS VALUES ('1','Monitor ASUS 21.5"', 'VP228HE-J Full HD 1ms HDMI VGA', '1', '1', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_27034_Monitor_ASUS_21.5__VP228HE-J_Full_HD_1ms_HDMI_VGA_a797ab9e-grn.jpg', '58650', '1', '10');</v>
       </c>
       <c r="L2">
         <v>1</v>
@@ -1371,8 +1371,8 @@
         <v>10</v>
       </c>
       <c r="K3" s="6" t="str">
-        <f t="shared" ref="K3:K63" si="0">CONCATENATE("INSERT INTO ARTICULOS VALUES ( '",C3, "', '", D3, "', '", E3, "', '", F3, "', '", G3, "', '", H3, "', '", I3, "', '", J3, "');")</f>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Monitor Gamer MSI 24"', 'Optix G241 144Hz IPS 1ms', '2', '1', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_20990_Monitor_Gamer_MSI_24__Optix_G241_144Hz_IPS_1ms_18f8b03a-grn.jpg', '119750', '1', '10');</v>
+        <f t="shared" ref="K3:K63" si="0">CONCATENATE("INSERT INTO ARTICULOS VALUES ('",B3, "','",C3, "', '", D3, "', '", E3, "', '", F3, "', '", G3, "', '", H3, "', '", I3, "', '", J3, "');")</f>
+        <v>INSERT INTO ARTICULOS VALUES ('2','Monitor Gamer MSI 24"', 'Optix G241 144Hz IPS 1ms', '2', '1', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_20990_Monitor_Gamer_MSI_24__Optix_G241_144Hz_IPS_1ms_18f8b03a-grn.jpg', '119750', '1', '10');</v>
       </c>
       <c r="L3">
         <v>2</v>
@@ -1419,7 +1419,7 @@
       </c>
       <c r="K4" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Monitor ASUS 24"', 'VA24EHE-J Full HD', '1', '1', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_33878_Monitor_ASUS_24__VA24EHE-J_Full_HD_ac877e59-grn.jpg', '77900', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('3','Monitor ASUS 24"', 'VA24EHE-J Full HD', '1', '1', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_33878_Monitor_ASUS_24__VA24EHE-J_Full_HD_ac877e59-grn.jpg', '77900', '1', '10');</v>
       </c>
       <c r="L4">
         <v>3</v>
@@ -1466,7 +1466,7 @@
       </c>
       <c r="K5" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Monitor ASUS 27"', ' Full HD HDMI VGA VA27EHE-J', '1', '1', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_33822_Monitor_ASUS_27__Full_HD_HDMI_VGA_VA27EHE-J_8b229ce8-grn.jpg', '60000', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('4','Monitor ASUS 27"', ' Full HD HDMI VGA VA27EHE-J', '1', '1', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_33822_Monitor_ASUS_27__Full_HD_HDMI_VGA_VA27EHE-J_8b229ce8-grn.jpg', '60000', '1', '10');</v>
       </c>
       <c r="L5">
         <v>4</v>
@@ -1513,7 +1513,7 @@
       </c>
       <c r="K6" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Monitor Gamer Viewsonic 24"', ' VX2468-PC-MHD Curvo 165hz', '11', '1', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_33359_Monitor_Gamer_Viewsonic_24__VX2468-PC-MHD_Curvo_165hz_46d27d6d-grn.jpg', '111500', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('5','Monitor Gamer Viewsonic 24"', ' VX2468-PC-MHD Curvo 165hz', '11', '1', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_33359_Monitor_Gamer_Viewsonic_24__VX2468-PC-MHD_Curvo_165hz_46d27d6d-grn.jpg', '111500', '1', '10');</v>
       </c>
       <c r="L6">
         <v>5</v>
@@ -1560,7 +1560,7 @@
       </c>
       <c r="K7" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Monitor Gamer Viewsonic 27"', 'VX2768 Curvo 2K 144Hz 1ms FreeSync HDMI DP', '11', '1', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_23822_Monitor_Gamer_Viewsonic_27__VX2768_Curvo_2K_144Hz_1ms_FreeSync_HDMI_DP_071c1138-grn.jpg', '207300', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('6','Monitor Gamer Viewsonic 27"', 'VX2768 Curvo 2K 144Hz 1ms FreeSync HDMI DP', '11', '1', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_23822_Monitor_Gamer_Viewsonic_27__VX2768_Curvo_2K_144Hz_1ms_FreeSync_HDMI_DP_071c1138-grn.jpg', '207300', '1', '10');</v>
       </c>
       <c r="L7">
         <v>6</v>
@@ -1606,7 +1606,7 @@
       </c>
       <c r="K8" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Placa de Video MSI GeForce RTX 3090', '24GB GDDR6X VENTUS 3X OC', '2', '2', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_36639_Placa_de_Video_MSI_GeForce_RTX_3090_24GB_GDDR6X_VENTUS_3X_OC_58618d16-grn.jpg', '443650', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('7','Placa de Video MSI GeForce RTX 3090', '24GB GDDR6X VENTUS 3X OC', '2', '2', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_36639_Placa_de_Video_MSI_GeForce_RTX_3090_24GB_GDDR6X_VENTUS_3X_OC_58618d16-grn.jpg', '443650', '1', '10');</v>
       </c>
       <c r="L8">
         <v>7</v>
@@ -1652,7 +1652,7 @@
       </c>
       <c r="K9" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Placa de Video ASUS Phoenix GeForce GTX 1630', '4GB GDDR6', '1', '2', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_36550_Placa_de_Video_ASUS_Phoenix_GeForce_GTX_1630_4GB_GDDR6_b0a0edd2-grn.jpg', '130000', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('8','Placa de Video ASUS Phoenix GeForce GTX 1630', '4GB GDDR6', '1', '2', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_36550_Placa_de_Video_ASUS_Phoenix_GeForce_GTX_1630_4GB_GDDR6_b0a0edd2-grn.jpg', '130000', '1', '10');</v>
       </c>
       <c r="L9">
         <v>8</v>
@@ -1698,7 +1698,7 @@
       </c>
       <c r="K10" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Placa de Video ASUS GeForce GTX 1660 SUPER', '6GB GDDR6 OC TUF', '1', '2', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_35211_Placa_de_Video_ASUS_GeForce_GTX_1660_SUPER_6GB_GDDR6_OC_TUF_91e6cd72-grn.jpg', '205000', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('9','Placa de Video ASUS GeForce GTX 1660 SUPER', '6GB GDDR6 OC TUF', '1', '2', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_35211_Placa_de_Video_ASUS_GeForce_GTX_1660_SUPER_6GB_GDDR6_OC_TUF_91e6cd72-grn.jpg', '205000', '1', '10');</v>
       </c>
       <c r="L10">
         <v>9</v>
@@ -1744,7 +1744,7 @@
       </c>
       <c r="K11" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Placa de Video ASUS GeForce GTX 1650', '4GB GDDR6 TUF GAMING', '1', '2', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_27548_Placa_de_Video_ASUS_GeForce_GTX_1650_4GB_GDDR6_TUF_GAMING_71e82ff4-grn.jpg', '190000', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('10','Placa de Video ASUS GeForce GTX 1650', '4GB GDDR6 TUF GAMING', '1', '2', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_27548_Placa_de_Video_ASUS_GeForce_GTX_1650_4GB_GDDR6_TUF_GAMING_71e82ff4-grn.jpg', '190000', '1', '10');</v>
       </c>
       <c r="L11">
         <v>10</v>
@@ -1790,7 +1790,7 @@
       </c>
       <c r="K12" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Placa de Video Asrock Radeon RX 550', '2GB GDDR5 Phantom Gaming', '11', '2', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_19289_Placa_de_Video_Asrock_Radeon_RX_550_2GB_GDDR5_Phantom_Gaming_99528ce8-grn.jpg', '58000', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('11','Placa de Video Asrock Radeon RX 550', '2GB GDDR5 Phantom Gaming', '11', '2', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_19289_Placa_de_Video_Asrock_Radeon_RX_550_2GB_GDDR5_Phantom_Gaming_99528ce8-grn.jpg', '58000', '1', '10');</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="17.25" x14ac:dyDescent="0.3">
@@ -1823,7 +1823,7 @@
       </c>
       <c r="K13" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Placa de Video Asrock Radeon RX 6800', 'XT 16GB GDDR6 Phantom Gaming D OC', '11', '2', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_29154_Placa_de_Video_Asrock_Radeon_RX_6800_XT_16GB_GDDR6_Phantom_Gaming_D_OC_b76349fe-grn.jpg', '283000', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('12','Placa de Video Asrock Radeon RX 6800', 'XT 16GB GDDR6 Phantom Gaming D OC', '11', '2', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_29154_Placa_de_Video_Asrock_Radeon_RX_6800_XT_16GB_GDDR6_Phantom_Gaming_D_OC_b76349fe-grn.jpg', '283000', '1', '10');</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="17.25" x14ac:dyDescent="0.3">
@@ -1856,7 +1856,7 @@
       </c>
       <c r="K14" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Disco Solido SSD M.2 WD 500GB Blue', 'SN570 3500MB/s NVMe PCI-E Gen3 x4 TLC', '9', '3', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_32107_Disco_Solido_SSD_M.2_WD_500GB_Blue_SN570_3500MB_s_NVMe_PCI-E_Gen3_x4_TLC_3135e1e9-grn.jpg', '27000', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('13','Disco Solido SSD M.2 WD 500GB Blue', 'SN570 3500MB/s NVMe PCI-E Gen3 x4 TLC', '9', '3', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_32107_Disco_Solido_SSD_M.2_WD_500GB_Blue_SN570_3500MB_s_NVMe_PCI-E_Gen3_x4_TLC_3135e1e9-grn.jpg', '27000', '1', '10');</v>
       </c>
       <c r="M14" s="2" t="s">
         <v>19</v>
@@ -1892,7 +1892,7 @@
       </c>
       <c r="K15" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Disco Solido SSD M.2 WD 500GB Black', 'SN750 SE 3600MB/s PCI-E X4 NVMe GEN4', '9', '3', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_28600_Disco_Solido_SSD_M.2_WD_500GB_Black_SN750_SE_3600MB_s_PCI-E_X4_NVMe_GEN4_b815bec0-grn.jpg', '31000', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('14','Disco Solido SSD M.2 WD 500GB Black', 'SN750 SE 3600MB/s PCI-E X4 NVMe GEN4', '9', '3', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_28600_Disco_Solido_SSD_M.2_WD_500GB_Black_SN750_SE_3600MB_s_PCI-E_X4_NVMe_GEN4_b815bec0-grn.jpg', '31000', '1', '10');</v>
       </c>
       <c r="L15">
         <v>1</v>
@@ -1938,7 +1938,7 @@
       </c>
       <c r="K16" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Disco Solido SSD M.2 WD 500GB WD_Black', 'SN770 5000MB/s NVMe PCI-E x4 Gen 4', '9', '3', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_33159_Disco_Solido_SSD_M.2_WD_500GB_WD_Black_SN770_5000MB_s_NVMe_PCI-E_x4_Gen_4_7a4a307b-grn.jpg', '42300', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('15','Disco Solido SSD M.2 WD 500GB WD_Black', 'SN770 5000MB/s NVMe PCI-E x4 Gen 4', '9', '3', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_33159_Disco_Solido_SSD_M.2_WD_500GB_WD_Black_SN770_5000MB_s_NVMe_PCI-E_x4_Gen_4_7a4a307b-grn.jpg', '42300', '1', '10');</v>
       </c>
       <c r="L16">
         <v>2</v>
@@ -1984,7 +1984,7 @@
       </c>
       <c r="K17" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Disco Solido SSD M.2 WD 1TB WD_Black SN770', '5150MB/s NVMe PCI-E x4 Gen 4', '9', '3', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_35589_Disco_Solido_SSD_M.2_WD_1TB_WD_Black_SN770_5150MB_s_NVMe_PCI-E_x4_Gen_4_7a4a307b-grn.jpg', '69000', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('16','Disco Solido SSD M.2 WD 1TB WD_Black SN770', '5150MB/s NVMe PCI-E x4 Gen 4', '9', '3', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_35589_Disco_Solido_SSD_M.2_WD_1TB_WD_Black_SN770_5150MB_s_NVMe_PCI-E_x4_Gen_4_7a4a307b-grn.jpg', '69000', '1', '10');</v>
       </c>
       <c r="L17">
         <v>3</v>
@@ -2030,7 +2030,7 @@
       </c>
       <c r="K18" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Disco Solido SSD Adata 240GB', 'SU650SS 520MB/s*', '12', '3', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_29777_Disco_Solido_SSD_Adata_240GB_SU650SS_520MB_s__8b455937-grn.jpg', '14000', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('17','Disco Solido SSD Adata 240GB', 'SU650SS 520MB/s*', '12', '3', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_29777_Disco_Solido_SSD_Adata_240GB_SU650SS_520MB_s__8b455937-grn.jpg', '14000', '1', '10');</v>
       </c>
       <c r="L18">
         <v>4</v>
@@ -2076,7 +2076,7 @@
       </c>
       <c r="K19" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Disco Rígido WD 1TB BLUE', '64MB SATA 6.0GB/s ', '9', '4', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_9018_Disco_R__gido_WD_1TB_BLUE_64MB_SATA_6.0GB_s__ca74d162-grn.jpg', '22000', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('18','Disco Rígido WD 1TB BLUE', '64MB SATA 6.0GB/s ', '9', '4', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_9018_Disco_R__gido_WD_1TB_BLUE_64MB_SATA_6.0GB_s__ca74d162-grn.jpg', '22000', '1', '10');</v>
       </c>
       <c r="L19">
         <v>5</v>
@@ -2122,7 +2122,7 @@
       </c>
       <c r="K20" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Disco Rigido WD 2TB BLUE', '256MB SATA 6.0GB/s', '9', '4', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_21014_Disco_Rigido_WD_2TB_BLUE_256MB_SATA_6.0GB_s_44f766ac-grn.jpg', '34000', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('19','Disco Rigido WD 2TB BLUE', '256MB SATA 6.0GB/s', '9', '4', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_21014_Disco_Rigido_WD_2TB_BLUE_256MB_SATA_6.0GB_s_44f766ac-grn.jpg', '34000', '1', '10');</v>
       </c>
       <c r="L20">
         <v>6</v>
@@ -2168,7 +2168,7 @@
       </c>
       <c r="K21" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Disco Rigido WD 2TB BLUE', '256MB SATA 6.0GB/s 7200RPM', '9', '4', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_35996_Disco_Rigido_WD_2TB_BLUE_256MB_SATA_6.0GB_s_7200RPM_dc36f8f5-grn.jpg', '34000', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('20','Disco Rigido WD 2TB BLUE', '256MB SATA 6.0GB/s 7200RPM', '9', '4', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_35996_Disco_Rigido_WD_2TB_BLUE_256MB_SATA_6.0GB_s_7200RPM_dc36f8f5-grn.jpg', '34000', '1', '10');</v>
       </c>
       <c r="L21">
         <v>7</v>
@@ -2214,7 +2214,7 @@
       </c>
       <c r="K22" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Disco Rigido WD 12TB Red', 'Pro 7.2K RPM 256MB', '9', '4', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_26480_Disco_Rigido_WD_12TB_Red_Pro_7.2K_RPM_256MB_c66a3fa3-grn.jpg', '126000', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('21','Disco Rigido WD 12TB Red', 'Pro 7.2K RPM 256MB', '9', '4', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_26480_Disco_Rigido_WD_12TB_Red_Pro_7.2K_RPM_256MB_c66a3fa3-grn.jpg', '126000', '1', '10');</v>
       </c>
       <c r="L22">
         <v>8</v>
@@ -2260,7 +2260,7 @@
       </c>
       <c r="K23" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Disco Rigido WD 12TB Gold', '7.2K RPM 256MB', '9', '4', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_26484_Disco_Rigido_WD_12TB_Gold_7.2K_RPM_256MB_856fe552-grn.jpg', '128000', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('22','Disco Rigido WD 12TB Gold', '7.2K RPM 256MB', '9', '4', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_26484_Disco_Rigido_WD_12TB_Gold_7.2K_RPM_256MB_856fe552-grn.jpg', '128000', '1', '10');</v>
       </c>
       <c r="L23">
         <v>9</v>
@@ -2306,7 +2306,7 @@
       </c>
       <c r="K24" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Memoria Adata DDR4 4GB', ' 2666MHz Value ', '12', '5', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_13221_Memoria_Adata_DDR4_4GB_2666MHz_Value__aa6df289-grn.jpg', '10500', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('23','Memoria Adata DDR4 4GB', ' 2666MHz Value ', '12', '5', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_13221_Memoria_Adata_DDR4_4GB_2666MHz_Value__aa6df289-grn.jpg', '10500', '1', '10');</v>
       </c>
       <c r="L24">
         <v>10</v>
@@ -2352,7 +2352,7 @@
       </c>
       <c r="K25" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Memoria Adata DDR4 8GB ', ' 2666MHz Value Sodimm Notebook', '12', '5', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_16184_Memoria_Adata_DDR4_8GB_2666MHz_Value_Sodimm_Notebook_38c2e2af-grn.jpg', '17000', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('24','Memoria Adata DDR4 8GB ', ' 2666MHz Value Sodimm Notebook', '12', '5', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_16184_Memoria_Adata_DDR4_8GB_2666MHz_Value_Sodimm_Notebook_38c2e2af-grn.jpg', '17000', '1', '10');</v>
       </c>
       <c r="L25">
         <v>11</v>
@@ -2398,7 +2398,7 @@
       </c>
       <c r="K26" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Memoria Adata DDR4 8GB', '3200MHz Premier', '12', '5', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_18814_Memoria_Adata_DDR4_8GB_3200MHz_Premier_c6036c27-grn.jpg', '19500', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('25','Memoria Adata DDR4 8GB', '3200MHz Premier', '12', '5', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_18814_Memoria_Adata_DDR4_8GB_3200MHz_Premier_c6036c27-grn.jpg', '19500', '1', '10');</v>
       </c>
       <c r="L26">
         <v>12</v>
@@ -2444,7 +2444,7 @@
       </c>
       <c r="K27" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Memoria Adata DDR4 16GB', '3200MHz CL16 XPG GAMMIX D20 Black', '12', '5', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_25890_Memoria_Adata_DDR4_16GB_3200MHz_CL16_XPG_GAMMIX_D20_Black_6b1582d3-grn.jpg', '43000', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('26','Memoria Adata DDR4 16GB', '3200MHz CL16 XPG GAMMIX D20 Black', '12', '5', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_25890_Memoria_Adata_DDR4_16GB_3200MHz_CL16_XPG_GAMMIX_D20_Black_6b1582d3-grn.jpg', '43000', '1', '10');</v>
       </c>
     </row>
     <row r="28" spans="2:15" ht="17.25" x14ac:dyDescent="0.3">
@@ -2477,7 +2477,7 @@
       </c>
       <c r="K28" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Memoria Adata DDR4 8GB ', '3200MHz XPG Spectrix D60G RGB Titanium', '12', '5', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_28924_Memoria_Adata_DDR4_8GB_3200MHz_XPG_Spectrix_D60G_RGB_Titanium_88f51e0f-grn.jpg', '21200', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('27','Memoria Adata DDR4 8GB ', '3200MHz XPG Spectrix D60G RGB Titanium', '12', '5', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_28924_Memoria_Adata_DDR4_8GB_3200MHz_XPG_Spectrix_D60G_RGB_Titanium_88f51e0f-grn.jpg', '21200', '1', '10');</v>
       </c>
     </row>
     <row r="29" spans="2:15" ht="17.25" x14ac:dyDescent="0.3">
@@ -2510,7 +2510,7 @@
       </c>
       <c r="K29" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Memoria Adata DDR4 8GB', '3200MHz XPG Spectrix D50 RGB Titanium', '12', '5', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_28926_Memoria_Adata_DDR4_8GB_3200MHz_XPG_Spectrix_D50_RGB_Titanium_446ebe28-grn.jpg', '25000', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('28','Memoria Adata DDR4 8GB', '3200MHz XPG Spectrix D50 RGB Titanium', '12', '5', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_28926_Memoria_Adata_DDR4_8GB_3200MHz_XPG_Spectrix_D50_RGB_Titanium_446ebe28-grn.jpg', '25000', '1', '10');</v>
       </c>
       <c r="M29" s="2" t="s">
         <v>50</v>
@@ -2546,7 +2546,7 @@
       </c>
       <c r="K30" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Memoria Adata DDR4 (2x8GB) 16GB ', '5000MHz XPG Spectrix D50 Xtreme RGB CL19', '12', '5', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_29885_Memoria_Adata_DDR4__2x8GB__16GB_5000MHz_XPG_Spectrix_D50_Xtreme_RGB_CL19_18133a6d-grn.jpg', '340000', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('29','Memoria Adata DDR4 (2x8GB) 16GB ', '5000MHz XPG Spectrix D50 Xtreme RGB CL19', '12', '5', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_29885_Memoria_Adata_DDR4__2x8GB__16GB_5000MHz_XPG_Spectrix_D50_Xtreme_RGB_CL19_18133a6d-grn.jpg', '340000', '1', '10');</v>
       </c>
       <c r="L30">
         <v>5</v>
@@ -2589,7 +2589,7 @@
       </c>
       <c r="K31" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Memoria Adata DDR4 8GB', '3600Mhz XPG Spectrix D45G RGB', '12', '5', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_29565_Memoria_Adata_DDR4_8GB_3600Mhz_XPG_Spectrix_D45G_RGB_cbbc726d-grn.jpg', '24500', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('30','Memoria Adata DDR4 8GB', '3600Mhz XPG Spectrix D45G RGB', '12', '5', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_29565_Memoria_Adata_DDR4_8GB_3600Mhz_XPG_Spectrix_D45G_RGB_cbbc726d-grn.jpg', '24500', '1', '10');</v>
       </c>
       <c r="L31">
         <v>5</v>
@@ -2632,7 +2632,7 @@
       </c>
       <c r="K32" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Teclado Mecanico Logitech PRO TKL', 'LOL 2 Switch Brown', '5', '6', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_33275_Teclado_Mecanico_Logitech_PRO_TKL_LOL_2_Switch_Brown_30e10b48-grn.jpg', '39000', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('31','Teclado Mecanico Logitech PRO TKL', 'LOL 2 Switch Brown', '5', '6', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_33275_Teclado_Mecanico_Logitech_PRO_TKL_LOL_2_Switch_Brown_30e10b48-grn.jpg', '39000', '1', '10');</v>
       </c>
       <c r="L32">
         <v>5</v>
@@ -2675,7 +2675,7 @@
       </c>
       <c r="K33" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Teclado Mecanico Logitech G513', 'Carbon RGB Switch GX Brown Español', '5', '6', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_19865_Teclado_Mecanico_Logitech_G513_Carbon_RGB_Switch_GX_Brown_Espa__ol_9ccf7c47-grn.jpg', '50000', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('32','Teclado Mecanico Logitech G513', 'Carbon RGB Switch GX Brown Español', '5', '6', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_19865_Teclado_Mecanico_Logitech_G513_Carbon_RGB_Switch_GX_Brown_Espa__ol_9ccf7c47-grn.jpg', '50000', '1', '10');</v>
       </c>
       <c r="L33">
         <v>6</v>
@@ -2718,7 +2718,7 @@
       </c>
       <c r="K34" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Teclado Mecanico Logitech POP Blast', 'Yellow Wireless', '5', '6', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_33269_Teclado_Mecanico_Logitech_POP_Blast_Yellow_Wireless_725996a0-grn.jpg', '52200', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('33','Teclado Mecanico Logitech POP Blast', 'Yellow Wireless', '5', '6', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_33269_Teclado_Mecanico_Logitech_POP_Blast_Yellow_Wireless_725996a0-grn.jpg', '52200', '1', '10');</v>
       </c>
       <c r="L34">
         <v>6</v>
@@ -2761,7 +2761,7 @@
       </c>
       <c r="K35" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Teclado Mecanico Logitech POP', 'Coral Rose Wireless', '5', '6', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_36665_Teclado_Mecanico_Logitech_POP_Coral_Rose_Wireless_065ab138-grn.jpg', '52000', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('34','Teclado Mecanico Logitech POP', 'Coral Rose Wireless', '5', '6', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_36665_Teclado_Mecanico_Logitech_POP_Coral_Rose_Wireless_065ab138-grn.jpg', '52000', '1', '10');</v>
       </c>
       <c r="L35">
         <v>2</v>
@@ -2804,7 +2804,7 @@
       </c>
       <c r="K36" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Teclado Logitech G815', 'Mechanical RGB Lightsync', '5', '6', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_16207_Teclado_Logitech_G815_Mechanical_RGB_Lightsync_5ab9b8b1-grn.jpg', '88000', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('35','Teclado Logitech G815', 'Mechanical RGB Lightsync', '5', '6', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_16207_Teclado_Logitech_G815_Mechanical_RGB_Lightsync_5ab9b8b1-grn.jpg', '88000', '1', '10');</v>
       </c>
       <c r="L36">
         <v>2</v>
@@ -2847,7 +2847,7 @@
       </c>
       <c r="K37" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Teclado Mecanico Logitech G915 TKL', 'RGB Lightspeed Inalambrico', '5', '6', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_19373_Teclado_Mecanico_Logitech_G915_TKL_RGB_Lightspeed_Inalambrico_065f0cec-grn.jpg', '115000', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('36','Teclado Mecanico Logitech G915 TKL', 'RGB Lightspeed Inalambrico', '5', '6', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_19373_Teclado_Mecanico_Logitech_G915_TKL_RGB_Lightspeed_Inalambrico_065f0cec-grn.jpg', '115000', '1', '10');</v>
       </c>
       <c r="L37">
         <v>2</v>
@@ -2887,7 +2887,7 @@
       </c>
       <c r="K38" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Teclado Mecanico Logitech Aurora G715', 'Wireless White RGB', '5', '6', '', '119000', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('37','Teclado Mecanico Logitech Aurora G715', 'Wireless White RGB', '5', '6', '', '119000', '1', '10');</v>
       </c>
       <c r="L38">
         <v>1</v>
@@ -2930,7 +2930,7 @@
       </c>
       <c r="K39" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Mouse Redragon Centrophorus ', 'M601 RGB', '6', '7', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_28612_Mouse_Redragon_Centrophorus_M601_RGB_e00743a5-grn.jpg', '7300', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('38','Mouse Redragon Centrophorus ', 'M601 RGB', '6', '7', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_28612_Mouse_Redragon_Centrophorus_M601_RGB_e00743a5-grn.jpg', '7300', '1', '10');</v>
       </c>
       <c r="L39">
         <v>1</v>
@@ -2973,7 +2973,7 @@
       </c>
       <c r="K40" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Mouse Redragon Mirage M690', '2.5GHz Wireless', '6', '7', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_8760_Mouse_Redragon_Mirage_M690_2.5GHz_Wireless_1739dc55-grn.jpg', '7500', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('39','Mouse Redragon Mirage M690', '2.5GHz Wireless', '6', '7', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_8760_Mouse_Redragon_Mirage_M690_2.5GHz_Wireless_1739dc55-grn.jpg', '7500', '1', '10');</v>
       </c>
       <c r="L40">
         <v>1</v>
@@ -3016,7 +3016,7 @@
       </c>
       <c r="K41" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Mouse Redragon Storm Elite M988', 'RGB Black', '6', '7', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_20297_Mouse_Redragon_Storm_Elite_M988_RGB_Black_f25e5643-grn.jpg', '13240', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('40','Mouse Redragon Storm Elite M988', 'RGB Black', '6', '7', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_20297_Mouse_Redragon_Storm_Elite_M988_RGB_Black_f25e5643-grn.jpg', '13240', '1', '10');</v>
       </c>
       <c r="L41">
         <v>3</v>
@@ -3059,7 +3059,7 @@
       </c>
       <c r="K42" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Mouse Logitech M110S', 'Negro Blue USB', '5', '7', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_18989_Mouse_Logitech_M110S_Negro_Blue_USB_9ecef8f4-grn.jpg', '3000', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('41','Mouse Logitech M110S', 'Negro Blue USB', '5', '7', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_18989_Mouse_Logitech_M110S_Negro_Blue_USB_9ecef8f4-grn.jpg', '3000', '1', '10');</v>
       </c>
       <c r="L42">
         <v>3</v>
@@ -3102,7 +3102,7 @@
       </c>
       <c r="K43" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Mouse Logitech M110S', 'Red Blue USB', '5', '7', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_24397_Mouse_Logitech_M110S_Red_520ace37-grn.jpg', '3000', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('42','Mouse Logitech M110S', 'Red Blue USB', '5', '7', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_24397_Mouse_Logitech_M110S_Red_520ace37-grn.jpg', '3000', '1', '10');</v>
       </c>
       <c r="L43">
         <v>3</v>
@@ -3145,7 +3145,7 @@
       </c>
       <c r="K44" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Mouse Logitech G305', 'Lightspeed Wireless Blue', '5', '7', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_21243_Mouse_Logitech_G305_Lightspeed_Wireless_Blue_9c250057-grn.jpg', '18600', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('43','Mouse Logitech G305', 'Lightspeed Wireless Blue', '5', '7', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_21243_Mouse_Logitech_G305_Lightspeed_Wireless_Blue_9c250057-grn.jpg', '18600', '1', '10');</v>
       </c>
       <c r="L44">
         <v>4</v>
@@ -3188,7 +3188,7 @@
       </c>
       <c r="K45" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Auriculares Redragon Zeus', 'RGB 7.1 Surround*', '6', '8', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_36399_Auriculares_Redragon_Zeus_X_H510-RGB_7.1_Surround__a5046a9f-grn.jpg', '32000', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('44','Auriculares Redragon Zeus', 'RGB 7.1 Surround*', '6', '8', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_36399_Auriculares_Redragon_Zeus_X_H510-RGB_7.1_Surround__a5046a9f-grn.jpg', '32000', '1', '10');</v>
       </c>
       <c r="L45">
         <v>4</v>
@@ -3231,7 +3231,7 @@
       </c>
       <c r="K46" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Auriculares Redragon Icon H520', 'PC PS4', '6', '8', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_29699_Auriculares_Redragon_Icon_H520_PC_PS4_42412af1-grn.jpg', '30000', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('45','Auriculares Redragon Icon H520', 'PC PS4', '6', '8', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_29699_Auriculares_Redragon_Icon_H520_PC_PS4_42412af1-grn.jpg', '30000', '1', '10');</v>
       </c>
       <c r="L46">
         <v>4</v>
@@ -3274,7 +3274,7 @@
       </c>
       <c r="K47" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Auriculares HP HyperX Cloud Stinger Gaming', 'Negro  PC | PS4 | Switch | XBOX', '7', '8', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_9612_Auriculares_HP_HyperX_Cloud_Stinger_Gaming_Negro__PC___PS4___Switch___XBOX_27f1808e-grn.jpg', '24200', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('46','Auriculares HP HyperX Cloud Stinger Gaming', 'Negro  PC | PS4 | Switch | XBOX', '7', '8', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_9612_Auriculares_HP_HyperX_Cloud_Stinger_Gaming_Negro__PC___PS4___Switch___XBOX_27f1808e-grn.jpg', '24200', '1', '10');</v>
       </c>
       <c r="L47">
         <v>7</v>
@@ -3317,7 +3317,7 @@
       </c>
       <c r="K48" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Auriculares HP HyperX Cloud', 'Black Blue PS4 PS5', '7', '8', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_35919_Auriculares_HP_HyperX_Cloud_Black_Blue_PS4_PS5_bdb54c92-grn.jpg', '32000', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('47','Auriculares HP HyperX Cloud', 'Black Blue PS4 PS5', '7', '8', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_35919_Auriculares_HP_HyperX_Cloud_Black_Blue_PS4_PS5_bdb54c92-grn.jpg', '32000', '1', '10');</v>
       </c>
       <c r="L48">
         <v>7</v>
@@ -3360,7 +3360,7 @@
       </c>
       <c r="K49" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Auriculares Genius GX', ' Gaming HS-G710V', '8', '8', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_31170_Auriculares_Genius_GX_Gaming_HS-G710V_e7832ba5-grn.jpg', '11000', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('48','Auriculares Genius GX', ' Gaming HS-G710V', '8', '8', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_31170_Auriculares_Genius_GX_Gaming_HS-G710V_e7832ba5-grn.jpg', '11000', '1', '10');</v>
       </c>
       <c r="L49">
         <v>7</v>
@@ -3403,7 +3403,7 @@
       </c>
       <c r="K50" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Auriculares Logitech G335', 'White', '5', '8', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_27936_Auriculares_Logitech_G335_White_32282a6d-grn.jpg', '22000', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('49','Auriculares Logitech G335', 'White', '5', '8', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_27936_Auriculares_Logitech_G335_White_32282a6d-grn.jpg', '22000', '1', '10');</v>
       </c>
       <c r="L50">
         <v>8</v>
@@ -3443,7 +3443,7 @@
       </c>
       <c r="K51" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Mother MSI A520M-A PRO AM4', '', '2', '9', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_21848_Mother_MSI_A520M-A_PRO_AM4_29d05f8c-grn.jpg', '55000', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('50','Mother MSI A520M-A PRO AM4', '', '2', '9', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_21848_Mother_MSI_A520M-A_PRO_AM4_29d05f8c-grn.jpg', '55000', '1', '10');</v>
       </c>
       <c r="L51">
         <v>8</v>
@@ -3483,7 +3483,7 @@
       </c>
       <c r="K52" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Mother ASUS PRIME A520M-K AM4', '', '1', '9', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_20551_Mother_ASUS_PRIME_A520M-K_AM4_f5d89e00-grn.jpg', '57750', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('51','Mother ASUS PRIME A520M-K AM4', '', '1', '9', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_20551_Mother_ASUS_PRIME_A520M-K_AM4_f5d89e00-grn.jpg', '57750', '1', '10');</v>
       </c>
       <c r="L52">
         <v>9</v>
@@ -3523,7 +3523,7 @@
       </c>
       <c r="K53" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Mother MSI B450 Gaming Plus Max AM4', '', '2', '9', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_25784_Mother_MSI_B450_Gaming_Plus_Max_AM4_5dd0dc29-grn.jpg', '71000', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('52','Mother MSI B450 Gaming Plus Max AM4', '', '2', '9', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_25784_Mother_MSI_B450_Gaming_Plus_Max_AM4_5dd0dc29-grn.jpg', '71000', '1', '10');</v>
       </c>
       <c r="L53">
         <v>9</v>
@@ -3563,7 +3563,7 @@
       </c>
       <c r="K54" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Mother MSI X570-A PRO AM4', '', '2', '9', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_15692_Mother_MSI_X570-A_PRO_AM4_bbf981bd-grn.jpg', '98000', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('53','Mother MSI X570-A PRO AM4', '', '2', '9', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_15692_Mother_MSI_X570-A_PRO_AM4_bbf981bd-grn.jpg', '98000', '1', '10');</v>
       </c>
       <c r="L54">
         <v>9</v>
@@ -3603,7 +3603,7 @@
       </c>
       <c r="K55" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Mother ASUS PRIME H610M-E D4 S1700', '', '1', '9', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_30440_Mother_ASUS_PRIME_H610M-E_D4_S1700_3402c168-grn.jpg', '53500', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('54','Mother ASUS PRIME H610M-E D4 S1700', '', '1', '9', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_30440_Mother_ASUS_PRIME_H610M-E_D4_S1700_3402c168-grn.jpg', '53500', '1', '10');</v>
       </c>
       <c r="L55">
         <v>10</v>
@@ -3643,7 +3643,7 @@
       </c>
       <c r="K56" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Mother Asrock H610M-HVS LGA 1700', '', '11', '9', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_34006_Mother_Asrock_H610M-HVS_LGA_1700_486791bd-grn.jpg', '53000', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('55','Mother Asrock H610M-HVS LGA 1700', '', '11', '9', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_34006_Mother_Asrock_H610M-HVS_LGA_1700_486791bd-grn.jpg', '53000', '1', '10');</v>
       </c>
       <c r="L56">
         <v>10</v>
@@ -3683,7 +3683,7 @@
       </c>
       <c r="K57" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Mother Asrock A520M-HDV AM4', '', '11', '9', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_24392_Mother_Asrock_A520M-HDV_AM4_5c7ae4d7-grn.jpg', '52000', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('56','Mother Asrock A520M-HDV AM4', '', '11', '9', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_24392_Mother_Asrock_A520M-HDV_AM4_5c7ae4d7-grn.jpg', '52000', '1', '10');</v>
       </c>
       <c r="L57">
         <v>11</v>
@@ -3726,7 +3726,7 @@
       </c>
       <c r="K58" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Procesador AMD RYZEN 5 3600', '4.2GHz Turbo AM4 Wraith Stealth Cooler', '3', '10', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_16749_Procesador_AMD_RYZEN_5_3600_4.2GHz_Turbo_AM4_Wraith_Stealth_Cooler_f8ab4915-grn.jpg', '94000', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('57','Procesador AMD RYZEN 5 3600', '4.2GHz Turbo AM4 Wraith Stealth Cooler', '3', '10', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_16749_Procesador_AMD_RYZEN_5_3600_4.2GHz_Turbo_AM4_Wraith_Stealth_Cooler_f8ab4915-grn.jpg', '94000', '1', '10');</v>
       </c>
       <c r="L58">
         <v>11</v>
@@ -3769,7 +3769,7 @@
       </c>
       <c r="K59" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Procesador AMD Ryzen 5 5500', '4.2GHz Turbo + Wraith Stealth Cooler', '3', '10', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_31696_Procesador_AMD_Ryzen_5_5500_4.2GHz_Turbo___Wraith_Stealth_Cooler_ca9fc7de-grn.jpg', '100000', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('58','Procesador AMD Ryzen 5 5500', '4.2GHz Turbo + Wraith Stealth Cooler', '3', '10', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_31696_Procesador_AMD_Ryzen_5_5500_4.2GHz_Turbo___Wraith_Stealth_Cooler_ca9fc7de-grn.jpg', '100000', '1', '10');</v>
       </c>
       <c r="L59">
         <v>12</v>
@@ -3812,7 +3812,7 @@
       </c>
       <c r="K60" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Procesador AMD Ryzen 9 5950X', '4.9GHz Turbo AM4 - No incluye Cooler', '3', '10', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_22302_Procesador_AMD_Ryzen_9_5950X_4.9GHz_Turbo_AM4_-_No_incluye_Cooler_9d34d3b3-grn.jpg', '250000', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('59','Procesador AMD Ryzen 9 5950X', '4.9GHz Turbo AM4 - No incluye Cooler', '3', '10', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_22302_Procesador_AMD_Ryzen_9_5950X_4.9GHz_Turbo_AM4_-_No_incluye_Cooler_9d34d3b3-grn.jpg', '250000', '1', '10');</v>
       </c>
       <c r="L60">
         <v>12</v>
@@ -3855,7 +3855,7 @@
       </c>
       <c r="K61" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Procesador Intel Pentium G4560', '3.5GHz Socket 1151 Kaby Lake OEM Sin Cooler', '4', '10', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_13151_Procesador_Intel_Pentium_G4560_3.5GHz_Socket_1151_Kaby_Lake_OEM_Sin_Cooler_58161f82-grn.jpg', '19000', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('60','Procesador Intel Pentium G4560', '3.5GHz Socket 1151 Kaby Lake OEM Sin Cooler', '4', '10', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_13151_Procesador_Intel_Pentium_G4560_3.5GHz_Socket_1151_Kaby_Lake_OEM_Sin_Cooler_58161f82-grn.jpg', '19000', '1', '10');</v>
       </c>
       <c r="L61">
         <v>12</v>
@@ -3898,7 +3898,7 @@
       </c>
       <c r="K62" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Procesador Intel Core i7 10700', '4.8GHz Turbo Socket 1200 Comet Lake', '4', '10', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_19228_Procesador_Intel_Core_i7_10700_4.8GHz_Turbo_Socket_1200_Comet_Lake_e3d7d847-grn.jpg', '191500', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('61','Procesador Intel Core i7 10700', '4.8GHz Turbo Socket 1200 Comet Lake', '4', '10', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_19228_Procesador_Intel_Core_i7_10700_4.8GHz_Turbo_Socket_1200_Comet_Lake_e3d7d847-grn.jpg', '191500', '1', '10');</v>
       </c>
       <c r="L62">
         <v>13</v>
@@ -3941,7 +3941,7 @@
       </c>
       <c r="K63" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ARTICULOS VALUES ( 'Procesador Intel Core i5 11600KF', '4.9GHz Turbo Socket 1200 Rocket Lake', '4', '10', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_25668_Procesador_Intel_Core_i5_11600KF_4.9GHz_Turbo_Socket_1200_Rocket_Lake_7f61810f-grn.jpg', '140000', '1', '10');</v>
+        <v>INSERT INTO ARTICULOS VALUES ('62','Procesador Intel Core i5 11600KF', '4.9GHz Turbo Socket 1200 Rocket Lake', '4', '10', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_25668_Procesador_Intel_Core_i5_11600KF_4.9GHz_Turbo_Socket_1200_Rocket_Lake_7f61810f-grn.jpg', '140000', '1', '10');</v>
       </c>
       <c r="L63">
         <v>13</v>

</xml_diff>

<commit_message>
agregado de validaciones y mejoras de funcionalidad en marcas y categorias
</commit_message>
<xml_diff>
--- a/Carga de datos.xlsx
+++ b/Carga de datos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manu\Desktop\TrabajoPracticoProgra\TPFinal-e19-Amarilla-Casulo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72342198-0B16-4014-BB9E-C684AC18C10E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B1797C-F27A-4313-8765-27CD010A3EC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -125,18 +125,6 @@
     <t>Western Digital</t>
   </si>
   <si>
-    <t>https://compragamer.net/imagenes_marcas/imagen_marca_364_9_203.jpg</t>
-  </si>
-  <si>
-    <t>https://compragamer.net/imagenes_marcas/imagen_marca_320_9_411.jpg</t>
-  </si>
-  <si>
-    <t>https://compragamer.net/imagenes_marcas/imagen_marca_365_9_441.jpg</t>
-  </si>
-  <si>
-    <t>https://compragamer.net/imagenes_marcas/imagen_marca_322_9_619.jpg</t>
-  </si>
-  <si>
     <t>https://styles.redditmedia.com/t5_42nhxk/styles/communityIcon_vb8305k77xo61.png?width=256&amp;s=7a4a763b7f929dd1ee7fe6ea04f9a27d71c581e0</t>
   </si>
   <si>
@@ -149,9 +137,6 @@
     <t>https://pbs.twimg.com/profile_images/674660612547432448/-mac6Il7_400x400.jpg</t>
   </si>
   <si>
-    <t>https://static.macupdate.com/products/62352/l/logitech-g-hub-logo.webp?v=1671137096</t>
-  </si>
-  <si>
     <t>https://cdn-icons-png.flaticon.com/256/81/81793.png</t>
   </si>
   <si>
@@ -185,9 +170,6 @@
     <t>ViewSonic</t>
   </si>
   <si>
-    <t>https://e7.pngegg.com/pngimages/466/107/png-clipart-hewlett-packard-viewsonic-computer-monitors-logo-computer-software-hewlett-packard-text-logo.png</t>
-  </si>
-  <si>
     <t>IMAGENES</t>
   </si>
   <si>
@@ -344,9 +326,6 @@
     <t>Asrock</t>
   </si>
   <si>
-    <t>https://cdn.shopify.com/s/files/1/0331/2789/1082/products/ASRock_grande.jpg?v=1582152086</t>
-  </si>
-  <si>
     <t>Placa de Video Asrock Radeon RX 550</t>
   </si>
   <si>
@@ -485,9 +464,6 @@
     <t>Adata</t>
   </si>
   <si>
-    <t>https://2.bp.blogspot.com/-yTiEnencHOA/T08JEEqNlKI/AAAAAAAABts/luVxNynFvW8/s1600/a6.jpg</t>
-  </si>
-  <si>
     <t>Memoria Adata DDR4 4GB</t>
   </si>
   <si>
@@ -873,6 +849,30 @@
   </si>
   <si>
     <t>https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_25668_Procesador_Intel_Core_i5_11600KF_4.9GHz_Turbo_Socket_1200_Rocket_Lake_7f61810f-grn.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn-icons-png.flaticon.com/512/731/731984.png</t>
+  </si>
+  <si>
+    <t>https://cdn-icons-png.flaticon.com/512/882/882700.png</t>
+  </si>
+  <si>
+    <t>https://cdn-icons-png.flaticon.com/512/882/882732.png</t>
+  </si>
+  <si>
+    <t>https://media.licdn.com/dms/image/C510BAQF5005y4n-01Q/company-logo_200_200/0/1519877464357?e=2147483647&amp;v=beta&amp;t=-K_JvIdI9NamxiWPSad3bUBfeM47UlrojmArlqbdf1s</t>
+  </si>
+  <si>
+    <t>https://www.westerndigital.com/content/dam/western-digital/en-us/portal-assets/logo/westerndigital-logo.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn.worldvectorlogo.com/logos/viewsonic.svg</t>
+  </si>
+  <si>
+    <t>https://pbs.twimg.com/profile_images/880260303572787201/yjCXDZRS_400x400.jpg</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/S/stores-image-uploads-eu-prod/1/AmazonStores/A1RKKUPIHCS9HS/5e2e5402ef2371c898414013c4e09e33.w400.h400.jpg</t>
   </si>
 </sst>
 </file>
@@ -940,7 +940,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -956,6 +956,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
@@ -1240,8 +1241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B38" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K68" sqref="K68"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1263,7 +1264,7 @@
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -1300,10 +1301,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
@@ -1312,7 +1313,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="H2" s="5">
         <v>58650</v>
@@ -1334,7 +1335,7 @@
         <v>9</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="O2" t="str">
         <f>CONCATENATE("INSERT INTO CATEGORIAS (id, descripcion, urlImagen) VALUES ('", L2, "', '", M2, "', '", TEXT(N2,"0"), "');")</f>
@@ -1347,10 +1348,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E3" s="1">
         <v>2</v>
@@ -1359,7 +1360,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H3" s="5">
         <v>119750</v>
@@ -1381,7 +1382,7 @@
         <v>10</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="O3" t="str">
         <f t="shared" ref="O3:O11" si="1">CONCATENATE("INSERT INTO CATEGORIAS (id, descripcion, urlImagen) VALUES ('", L3, "', '", M3, "', '", TEXT(N3,"0"), "');")</f>
@@ -1394,10 +1395,10 @@
         <v>3</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
@@ -1406,7 +1407,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="H4" s="5">
         <v>77900</v>
@@ -1428,7 +1429,7 @@
         <v>11</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="O4" t="str">
         <f t="shared" si="1"/>
@@ -1441,10 +1442,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E5" s="1">
         <v>1</v>
@@ -1453,7 +1454,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="H5" s="5">
         <v>60000</v>
@@ -1475,7 +1476,7 @@
         <v>12</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="O5" t="str">
         <f t="shared" si="1"/>
@@ -1488,10 +1489,10 @@
         <v>5</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E6" s="1">
         <v>11</v>
@@ -1500,7 +1501,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="H6" s="5">
         <v>111500</v>
@@ -1522,7 +1523,7 @@
         <v>13</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="O6" t="str">
         <f t="shared" si="1"/>
@@ -1535,10 +1536,10 @@
         <v>6</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E7" s="1">
         <v>11</v>
@@ -1547,7 +1548,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="H7" s="5">
         <v>207300</v>
@@ -1569,7 +1570,7 @@
         <v>14</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="O7" t="str">
         <f t="shared" si="1"/>
@@ -1581,10 +1582,10 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D8" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E8" s="1">
         <v>2</v>
@@ -1593,7 +1594,7 @@
         <v>2</v>
       </c>
       <c r="G8" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="H8" s="5">
         <v>443650</v>
@@ -1615,7 +1616,7 @@
         <v>15</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="O8" t="str">
         <f t="shared" si="1"/>
@@ -1627,10 +1628,10 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D9" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E9" s="1">
         <v>1</v>
@@ -1639,7 +1640,7 @@
         <v>2</v>
       </c>
       <c r="G9" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="H9" s="5">
         <v>130000</v>
@@ -1661,7 +1662,7 @@
         <v>16</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="O9" t="str">
         <f t="shared" si="1"/>
@@ -1673,10 +1674,10 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D10" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
@@ -1685,7 +1686,7 @@
         <v>2</v>
       </c>
       <c r="G10" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H10" s="5">
         <v>205000</v>
@@ -1707,7 +1708,7 @@
         <v>17</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="O10" t="str">
         <f t="shared" si="1"/>
@@ -1719,10 +1720,10 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D11" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
@@ -1731,7 +1732,7 @@
         <v>2</v>
       </c>
       <c r="G11" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="H11" s="5">
         <v>190000</v>
@@ -1753,7 +1754,7 @@
         <v>18</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="O11" t="str">
         <f t="shared" si="1"/>
@@ -1765,10 +1766,10 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D12" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="E12" s="1">
         <v>11</v>
@@ -1777,7 +1778,7 @@
         <v>2</v>
       </c>
       <c r="G12" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="H12" s="5">
         <v>58000</v>
@@ -1798,10 +1799,10 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D13" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="E13" s="1">
         <v>11</v>
@@ -1810,7 +1811,7 @@
         <v>2</v>
       </c>
       <c r="G13" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="H13" s="5">
         <v>283000</v>
@@ -1831,10 +1832,10 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="D14" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="E14" s="1">
         <v>9</v>
@@ -1843,7 +1844,7 @@
         <v>3</v>
       </c>
       <c r="G14" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="H14" s="5">
         <v>27000</v>
@@ -1867,10 +1868,10 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="D15" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="E15" s="1">
         <v>9</v>
@@ -1879,7 +1880,7 @@
         <v>3</v>
       </c>
       <c r="G15" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="H15" s="5">
         <v>31000</v>
@@ -1901,7 +1902,7 @@
         <v>20</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="O15" t="str">
         <f>CONCATENATE("INSERT INTO MARCAS (id, descripcion, urlImagen) VALUES ('", L15, "', '", M15, "', '", TEXT(N15,"0"), "');")</f>
@@ -1913,10 +1914,10 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D16" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="E16" s="1">
         <v>9</v>
@@ -1925,7 +1926,7 @@
         <v>3</v>
       </c>
       <c r="G16" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="H16" s="5">
         <v>42300</v>
@@ -1947,7 +1948,7 @@
         <v>21</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="O16" t="str">
         <f t="shared" ref="O16:O26" si="2">CONCATENATE("INSERT INTO MARCAS (id, descripcion, urlImagen) VALUES ('", L16, "', '", M16, "', '", TEXT(N16,"0"), "');")</f>
@@ -1959,10 +1960,10 @@
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D17" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="E17" s="1">
         <v>9</v>
@@ -1971,7 +1972,7 @@
         <v>3</v>
       </c>
       <c r="G17" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="H17" s="5">
         <v>69000</v>
@@ -1993,11 +1994,11 @@
         <v>22</v>
       </c>
       <c r="N17" s="3" t="s">
-        <v>30</v>
+        <v>271</v>
       </c>
       <c r="O17" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO MARCAS (id, descripcion, urlImagen) VALUES ('3', 'Amd', 'https://compragamer.net/imagenes_marcas/imagen_marca_320_9_411.jpg');</v>
+        <v>INSERT INTO MARCAS (id, descripcion, urlImagen) VALUES ('3', 'Amd', 'https://cdn-icons-png.flaticon.com/512/731/731984.png');</v>
       </c>
     </row>
     <row r="18" spans="2:15" ht="17.25" x14ac:dyDescent="0.3">
@@ -2005,10 +2006,10 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D18" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E18" s="1">
         <v>12</v>
@@ -2017,7 +2018,7 @@
         <v>3</v>
       </c>
       <c r="G18" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="H18" s="5">
         <v>14000</v>
@@ -2039,11 +2040,11 @@
         <v>23</v>
       </c>
       <c r="N18" s="3" t="s">
-        <v>29</v>
+        <v>272</v>
       </c>
       <c r="O18" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO MARCAS (id, descripcion, urlImagen) VALUES ('4', 'Intel', 'https://compragamer.net/imagenes_marcas/imagen_marca_364_9_203.jpg');</v>
+        <v>INSERT INTO MARCAS (id, descripcion, urlImagen) VALUES ('4', 'Intel', 'https://cdn-icons-png.flaticon.com/512/882/882700.png');</v>
       </c>
     </row>
     <row r="19" spans="2:15" ht="17.25" x14ac:dyDescent="0.3">
@@ -2051,10 +2052,10 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="D19" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="E19" s="1">
         <v>9</v>
@@ -2063,7 +2064,7 @@
         <v>4</v>
       </c>
       <c r="G19" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="H19" s="5">
         <v>22000</v>
@@ -2085,11 +2086,11 @@
         <v>24</v>
       </c>
       <c r="N19" s="3" t="s">
-        <v>37</v>
+        <v>273</v>
       </c>
       <c r="O19" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO MARCAS (id, descripcion, urlImagen) VALUES ('5', 'Logitech', 'https://static.macupdate.com/products/62352/l/logitech-g-hub-logo.webp?v=1671137096');</v>
+        <v>INSERT INTO MARCAS (id, descripcion, urlImagen) VALUES ('5', 'Logitech', 'https://cdn-icons-png.flaticon.com/512/882/882732.png');</v>
       </c>
     </row>
     <row r="20" spans="2:15" ht="17.25" x14ac:dyDescent="0.3">
@@ -2097,10 +2098,10 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D20" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="E20" s="1">
         <v>9</v>
@@ -2109,7 +2110,7 @@
         <v>4</v>
       </c>
       <c r="G20" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="H20" s="5">
         <v>34000</v>
@@ -2131,7 +2132,7 @@
         <v>25</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="O20" t="str">
         <f t="shared" si="2"/>
@@ -2143,10 +2144,10 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D21" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="E21" s="1">
         <v>9</v>
@@ -2155,7 +2156,7 @@
         <v>4</v>
       </c>
       <c r="G21" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="H21" s="5">
         <v>34000</v>
@@ -2177,11 +2178,11 @@
         <v>26</v>
       </c>
       <c r="N21" s="3" t="s">
-        <v>31</v>
+        <v>274</v>
       </c>
       <c r="O21" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO MARCAS (id, descripcion, urlImagen) VALUES ('7', 'HyperX', 'https://compragamer.net/imagenes_marcas/imagen_marca_365_9_441.jpg');</v>
+        <v>INSERT INTO MARCAS (id, descripcion, urlImagen) VALUES ('7', 'HyperX', 'https://media.licdn.com/dms/image/C510BAQF5005y4n-01Q/company-logo_200_200/0/1519877464357?e=2147483647&amp;v=beta&amp;t=-K_JvIdI9NamxiWPSad3bUBfeM47UlrojmArlqbdf1s');</v>
       </c>
     </row>
     <row r="22" spans="2:15" ht="17.25" x14ac:dyDescent="0.3">
@@ -2189,10 +2190,10 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="D22" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="E22" s="1">
         <v>9</v>
@@ -2201,7 +2202,7 @@
         <v>4</v>
       </c>
       <c r="G22" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="H22" s="5">
         <v>126000</v>
@@ -2223,7 +2224,7 @@
         <v>27</v>
       </c>
       <c r="N22" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="O22" t="str">
         <f t="shared" si="2"/>
@@ -2235,10 +2236,10 @@
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="D23" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="E23" s="1">
         <v>9</v>
@@ -2247,7 +2248,7 @@
         <v>4</v>
       </c>
       <c r="G23" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="H23" s="5">
         <v>128000</v>
@@ -2269,11 +2270,11 @@
         <v>28</v>
       </c>
       <c r="N23" s="3" t="s">
-        <v>32</v>
+        <v>275</v>
       </c>
       <c r="O23" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO MARCAS (id, descripcion, urlImagen) VALUES ('9', 'Western Digital', 'https://compragamer.net/imagenes_marcas/imagen_marca_322_9_619.jpg');</v>
+        <v>INSERT INTO MARCAS (id, descripcion, urlImagen) VALUES ('9', 'Western Digital', 'https://www.westerndigital.com/content/dam/western-digital/en-us/portal-assets/logo/westerndigital-logo.jpg');</v>
       </c>
     </row>
     <row r="24" spans="2:15" ht="17.25" x14ac:dyDescent="0.3">
@@ -2281,10 +2282,10 @@
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D24" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="E24" s="1">
         <v>12</v>
@@ -2293,7 +2294,7 @@
         <v>5</v>
       </c>
       <c r="G24" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="H24" s="5">
         <v>10500</v>
@@ -2312,14 +2313,14 @@
         <v>10</v>
       </c>
       <c r="M24" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="N24" s="3" t="s">
-        <v>49</v>
+        <v>276</v>
       </c>
       <c r="O24" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO MARCAS (id, descripcion, urlImagen) VALUES ('10', 'ViewSonic', 'https://e7.pngegg.com/pngimages/466/107/png-clipart-hewlett-packard-viewsonic-computer-monitors-logo-computer-software-hewlett-packard-text-logo.png');</v>
+        <v>INSERT INTO MARCAS (id, descripcion, urlImagen) VALUES ('10', 'ViewSonic', 'https://cdn.worldvectorlogo.com/logos/viewsonic.svg');</v>
       </c>
     </row>
     <row r="25" spans="2:15" ht="17.25" x14ac:dyDescent="0.3">
@@ -2327,10 +2328,10 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="D25" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="E25" s="1">
         <v>12</v>
@@ -2339,7 +2340,7 @@
         <v>5</v>
       </c>
       <c r="G25" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="H25" s="5">
         <v>17000</v>
@@ -2358,14 +2359,14 @@
         <v>11</v>
       </c>
       <c r="M25" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="N25" t="s">
-        <v>102</v>
+        <v>277</v>
       </c>
       <c r="O25" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO MARCAS (id, descripcion, urlImagen) VALUES ('11', 'Asrock', 'https://cdn.shopify.com/s/files/1/0331/2789/1082/products/ASRock_grande.jpg?v=1582152086');</v>
+        <v>INSERT INTO MARCAS (id, descripcion, urlImagen) VALUES ('11', 'Asrock', 'https://pbs.twimg.com/profile_images/880260303572787201/yjCXDZRS_400x400.jpg');</v>
       </c>
     </row>
     <row r="26" spans="2:15" ht="17.25" x14ac:dyDescent="0.3">
@@ -2373,10 +2374,10 @@
         <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D26" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="E26" s="1">
         <v>12</v>
@@ -2385,7 +2386,7 @@
         <v>5</v>
       </c>
       <c r="G26" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="H26" s="5">
         <v>19500</v>
@@ -2404,14 +2405,14 @@
         <v>12</v>
       </c>
       <c r="M26" t="s">
-        <v>148</v>
-      </c>
-      <c r="N26" t="s">
-        <v>149</v>
+        <v>141</v>
+      </c>
+      <c r="N26" s="7" t="s">
+        <v>278</v>
       </c>
       <c r="O26" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO MARCAS (id, descripcion, urlImagen) VALUES ('12', 'Adata', 'https://2.bp.blogspot.com/-yTiEnencHOA/T08JEEqNlKI/AAAAAAAABts/luVxNynFvW8/s1600/a6.jpg');</v>
+        <v>INSERT INTO MARCAS (id, descripcion, urlImagen) VALUES ('12', 'Adata', 'https://m.media-amazon.com/images/S/stores-image-uploads-eu-prod/1/AmazonStores/A1RKKUPIHCS9HS/5e2e5402ef2371c898414013c4e09e33.w400.h400.jpg');</v>
       </c>
     </row>
     <row r="27" spans="2:15" ht="17.25" x14ac:dyDescent="0.3">
@@ -2419,10 +2420,10 @@
         <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D27" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="E27" s="1">
         <v>12</v>
@@ -2431,7 +2432,7 @@
         <v>5</v>
       </c>
       <c r="G27" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="H27" s="5">
         <v>43000</v>
@@ -2452,10 +2453,10 @@
         <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="D28" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="E28" s="1">
         <v>12</v>
@@ -2464,7 +2465,7 @@
         <v>5</v>
       </c>
       <c r="G28" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="H28" s="5">
         <v>21200</v>
@@ -2485,10 +2486,10 @@
         <v>28</v>
       </c>
       <c r="C29" t="s">
+        <v>148</v>
+      </c>
+      <c r="D29" t="s">
         <v>156</v>
-      </c>
-      <c r="D29" t="s">
-        <v>164</v>
       </c>
       <c r="E29" s="1">
         <v>12</v>
@@ -2497,7 +2498,7 @@
         <v>5</v>
       </c>
       <c r="G29" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="H29" s="5">
         <v>25000</v>
@@ -2513,7 +2514,7 @@
         <v>INSERT INTO ARTICULOS VALUES ('28','Memoria Adata DDR4 8GB', '3200MHz XPG Spectrix D50 RGB Titanium', '12', '5', 'https://compragamer.net/pga/imagenes_publicadas/compragamer_Imganen_general_28926_Memoria_Adata_DDR4_8GB_3200MHz_XPG_Spectrix_D50_RGB_Titanium_446ebe28-grn.jpg', '25000', '1', '10');</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="2:15" ht="17.25" x14ac:dyDescent="0.3">
@@ -2521,10 +2522,10 @@
         <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="D30" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="E30" s="1">
         <v>12</v>
@@ -2533,7 +2534,7 @@
         <v>5</v>
       </c>
       <c r="G30" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="H30" s="5">
         <v>340000</v>
@@ -2552,7 +2553,7 @@
         <v>5</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="N30" t="str">
         <f>CONCATENATE("INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('", L30, "','", TEXT(M30,"0"), "');")</f>
@@ -2564,10 +2565,10 @@
         <v>30</v>
       </c>
       <c r="C31" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D31" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="E31" s="1">
         <v>12</v>
@@ -2576,7 +2577,7 @@
         <v>5</v>
       </c>
       <c r="G31" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="H31" s="5">
         <v>24500</v>
@@ -2595,7 +2596,7 @@
         <v>5</v>
       </c>
       <c r="M31" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="N31" t="str">
         <f t="shared" ref="N31:N94" si="3">CONCATENATE("INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('", L31, "','", TEXT(M31,"0"), "');")</f>
@@ -2607,10 +2608,10 @@
         <v>31</v>
       </c>
       <c r="C32" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="D32" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E32" s="1">
         <v>5</v>
@@ -2619,7 +2620,7 @@
         <v>6</v>
       </c>
       <c r="G32" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="H32" s="5">
         <v>39000</v>
@@ -2638,7 +2639,7 @@
         <v>5</v>
       </c>
       <c r="M32" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="N32" t="str">
         <f t="shared" si="3"/>
@@ -2650,10 +2651,10 @@
         <v>32</v>
       </c>
       <c r="C33" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="D33" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="E33" s="1">
         <v>5</v>
@@ -2662,7 +2663,7 @@
         <v>6</v>
       </c>
       <c r="G33" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="H33" s="5">
         <v>50000</v>
@@ -2681,7 +2682,7 @@
         <v>6</v>
       </c>
       <c r="M33" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="N33" t="str">
         <f t="shared" si="3"/>
@@ -2693,10 +2694,10 @@
         <v>33</v>
       </c>
       <c r="C34" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="D34" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="E34" s="1">
         <v>5</v>
@@ -2705,7 +2706,7 @@
         <v>6</v>
       </c>
       <c r="G34" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="H34" s="5">
         <v>52200</v>
@@ -2724,7 +2725,7 @@
         <v>6</v>
       </c>
       <c r="M34" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="N34" t="str">
         <f t="shared" si="3"/>
@@ -2736,10 +2737,10 @@
         <v>34</v>
       </c>
       <c r="C35" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D35" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="E35" s="1">
         <v>5</v>
@@ -2748,7 +2749,7 @@
         <v>6</v>
       </c>
       <c r="G35" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="H35" s="5">
         <v>52000</v>
@@ -2767,7 +2768,7 @@
         <v>2</v>
       </c>
       <c r="M35" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="N35" t="str">
         <f t="shared" si="3"/>
@@ -2779,10 +2780,10 @@
         <v>35</v>
       </c>
       <c r="C36" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="D36" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="E36" s="1">
         <v>5</v>
@@ -2791,7 +2792,7 @@
         <v>6</v>
       </c>
       <c r="G36" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="H36" s="5">
         <v>88000</v>
@@ -2810,7 +2811,7 @@
         <v>2</v>
       </c>
       <c r="M36" s="3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="N36" t="str">
         <f t="shared" si="3"/>
@@ -2822,10 +2823,10 @@
         <v>36</v>
       </c>
       <c r="C37" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="D37" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E37" s="1">
         <v>5</v>
@@ -2834,7 +2835,7 @@
         <v>6</v>
       </c>
       <c r="G37" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="H37" s="5">
         <v>115000</v>
@@ -2853,7 +2854,7 @@
         <v>2</v>
       </c>
       <c r="M37" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="N37" t="str">
         <f t="shared" si="3"/>
@@ -2865,10 +2866,10 @@
         <v>37</v>
       </c>
       <c r="C38" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="D38" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="E38" s="1">
         <v>5</v>
@@ -2893,7 +2894,7 @@
         <v>1</v>
       </c>
       <c r="M38" s="3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="N38" t="str">
         <f t="shared" si="3"/>
@@ -2905,10 +2906,10 @@
         <v>38</v>
       </c>
       <c r="C39" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="D39" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="E39" s="1">
         <v>6</v>
@@ -2917,7 +2918,7 @@
         <v>7</v>
       </c>
       <c r="G39" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="H39" s="5">
         <v>7300</v>
@@ -2936,7 +2937,7 @@
         <v>1</v>
       </c>
       <c r="M39" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="N39" t="str">
         <f t="shared" si="3"/>
@@ -2948,10 +2949,10 @@
         <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="D40" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="E40" s="1">
         <v>6</v>
@@ -2960,7 +2961,7 @@
         <v>7</v>
       </c>
       <c r="G40" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="H40" s="5">
         <v>7500</v>
@@ -2979,7 +2980,7 @@
         <v>1</v>
       </c>
       <c r="M40" s="3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="N40" t="str">
         <f t="shared" si="3"/>
@@ -2991,10 +2992,10 @@
         <v>40</v>
       </c>
       <c r="C41" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="D41" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="E41" s="1">
         <v>6</v>
@@ -3003,7 +3004,7 @@
         <v>7</v>
       </c>
       <c r="G41" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="H41" s="5">
         <v>13240</v>
@@ -3022,7 +3023,7 @@
         <v>3</v>
       </c>
       <c r="M41" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="N41" t="str">
         <f t="shared" si="3"/>
@@ -3034,10 +3035,10 @@
         <v>41</v>
       </c>
       <c r="C42" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="D42" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="E42" s="1">
         <v>5</v>
@@ -3046,7 +3047,7 @@
         <v>7</v>
       </c>
       <c r="G42" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="H42" s="5">
         <v>3000</v>
@@ -3065,7 +3066,7 @@
         <v>3</v>
       </c>
       <c r="M42" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="N42" t="str">
         <f t="shared" si="3"/>
@@ -3077,10 +3078,10 @@
         <v>42</v>
       </c>
       <c r="C43" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="D43" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="E43" s="1">
         <v>5</v>
@@ -3089,7 +3090,7 @@
         <v>7</v>
       </c>
       <c r="G43" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="H43" s="5">
         <v>3000</v>
@@ -3108,7 +3109,7 @@
         <v>3</v>
       </c>
       <c r="M43" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="N43" t="str">
         <f t="shared" si="3"/>
@@ -3120,10 +3121,10 @@
         <v>43</v>
       </c>
       <c r="C44" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="D44" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="E44" s="1">
         <v>5</v>
@@ -3132,7 +3133,7 @@
         <v>7</v>
       </c>
       <c r="G44" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="H44" s="5">
         <v>18600</v>
@@ -3151,7 +3152,7 @@
         <v>4</v>
       </c>
       <c r="M44" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="N44" t="str">
         <f t="shared" si="3"/>
@@ -3163,10 +3164,10 @@
         <v>44</v>
       </c>
       <c r="C45" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="D45" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="E45" s="1">
         <v>6</v>
@@ -3175,7 +3176,7 @@
         <v>8</v>
       </c>
       <c r="G45" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="H45" s="5">
         <v>32000</v>
@@ -3194,7 +3195,7 @@
         <v>4</v>
       </c>
       <c r="M45" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="N45" t="str">
         <f t="shared" si="3"/>
@@ -3206,10 +3207,10 @@
         <v>45</v>
       </c>
       <c r="C46" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="D46" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="E46" s="1">
         <v>6</v>
@@ -3218,7 +3219,7 @@
         <v>8</v>
       </c>
       <c r="G46" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="H46" s="5">
         <v>30000</v>
@@ -3237,7 +3238,7 @@
         <v>4</v>
       </c>
       <c r="M46" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="N46" t="str">
         <f t="shared" si="3"/>
@@ -3249,10 +3250,10 @@
         <v>46</v>
       </c>
       <c r="C47" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="D47" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="E47" s="1">
         <v>7</v>
@@ -3261,7 +3262,7 @@
         <v>8</v>
       </c>
       <c r="G47" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="H47" s="5">
         <v>24200</v>
@@ -3280,7 +3281,7 @@
         <v>7</v>
       </c>
       <c r="M47" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="N47" t="str">
         <f t="shared" si="3"/>
@@ -3292,10 +3293,10 @@
         <v>47</v>
       </c>
       <c r="C48" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="D48" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="E48" s="1">
         <v>7</v>
@@ -3304,7 +3305,7 @@
         <v>8</v>
       </c>
       <c r="G48" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="H48" s="5">
         <v>32000</v>
@@ -3323,7 +3324,7 @@
         <v>7</v>
       </c>
       <c r="M48" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="N48" t="str">
         <f t="shared" si="3"/>
@@ -3335,10 +3336,10 @@
         <v>48</v>
       </c>
       <c r="C49" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="D49" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="E49" s="1">
         <v>8</v>
@@ -3347,7 +3348,7 @@
         <v>8</v>
       </c>
       <c r="G49" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="H49" s="5">
         <v>11000</v>
@@ -3366,7 +3367,7 @@
         <v>7</v>
       </c>
       <c r="M49" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="N49" t="str">
         <f t="shared" si="3"/>
@@ -3378,10 +3379,10 @@
         <v>49</v>
       </c>
       <c r="C50" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="D50" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="E50" s="1">
         <v>5</v>
@@ -3390,7 +3391,7 @@
         <v>8</v>
       </c>
       <c r="G50" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="H50" s="5">
         <v>22000</v>
@@ -3409,7 +3410,7 @@
         <v>8</v>
       </c>
       <c r="M50" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="N50" t="str">
         <f t="shared" si="3"/>
@@ -3421,7 +3422,7 @@
         <v>50</v>
       </c>
       <c r="C51" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="E51" s="1">
         <v>2</v>
@@ -3430,7 +3431,7 @@
         <v>9</v>
       </c>
       <c r="G51" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="H51" s="5">
         <v>55000</v>
@@ -3449,7 +3450,7 @@
         <v>8</v>
       </c>
       <c r="M51" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="N51" t="str">
         <f t="shared" si="3"/>
@@ -3461,7 +3462,7 @@
         <v>51</v>
       </c>
       <c r="C52" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="E52" s="1">
         <v>1</v>
@@ -3470,7 +3471,7 @@
         <v>9</v>
       </c>
       <c r="G52" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="H52" s="5">
         <v>57750</v>
@@ -3489,7 +3490,7 @@
         <v>9</v>
       </c>
       <c r="M52" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="N52" t="str">
         <f t="shared" si="3"/>
@@ -3501,7 +3502,7 @@
         <v>52</v>
       </c>
       <c r="C53" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="E53" s="1">
         <v>2</v>
@@ -3510,7 +3511,7 @@
         <v>9</v>
       </c>
       <c r="G53" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="H53" s="5">
         <v>71000</v>
@@ -3529,7 +3530,7 @@
         <v>9</v>
       </c>
       <c r="M53" s="3" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="N53" t="str">
         <f t="shared" si="3"/>
@@ -3541,7 +3542,7 @@
         <v>53</v>
       </c>
       <c r="C54" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="E54" s="1">
         <v>2</v>
@@ -3550,7 +3551,7 @@
         <v>9</v>
       </c>
       <c r="G54" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="H54" s="5">
         <v>98000</v>
@@ -3569,7 +3570,7 @@
         <v>9</v>
       </c>
       <c r="M54" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="N54" t="str">
         <f t="shared" si="3"/>
@@ -3581,7 +3582,7 @@
         <v>54</v>
       </c>
       <c r="C55" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E55" s="1">
         <v>1</v>
@@ -3590,7 +3591,7 @@
         <v>9</v>
       </c>
       <c r="G55" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="H55" s="5">
         <v>53500</v>
@@ -3609,7 +3610,7 @@
         <v>10</v>
       </c>
       <c r="M55" s="3" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="N55" t="str">
         <f t="shared" si="3"/>
@@ -3621,7 +3622,7 @@
         <v>55</v>
       </c>
       <c r="C56" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="E56" s="1">
         <v>11</v>
@@ -3630,7 +3631,7 @@
         <v>9</v>
       </c>
       <c r="G56" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H56" s="5">
         <v>53000</v>
@@ -3649,7 +3650,7 @@
         <v>10</v>
       </c>
       <c r="M56" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="N56" t="str">
         <f t="shared" si="3"/>
@@ -3661,7 +3662,7 @@
         <v>56</v>
       </c>
       <c r="C57" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="E57" s="1">
         <v>11</v>
@@ -3670,7 +3671,7 @@
         <v>9</v>
       </c>
       <c r="G57" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="H57" s="5">
         <v>52000</v>
@@ -3689,7 +3690,7 @@
         <v>11</v>
       </c>
       <c r="M57" s="3" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="N57" t="str">
         <f t="shared" si="3"/>
@@ -3701,10 +3702,10 @@
         <v>57</v>
       </c>
       <c r="C58" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="D58" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="E58" s="1">
         <v>3</v>
@@ -3713,7 +3714,7 @@
         <v>10</v>
       </c>
       <c r="G58" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="H58" s="5">
         <v>94000</v>
@@ -3732,7 +3733,7 @@
         <v>11</v>
       </c>
       <c r="M58" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="N58" t="str">
         <f t="shared" si="3"/>
@@ -3744,10 +3745,10 @@
         <v>58</v>
       </c>
       <c r="C59" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="D59" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="E59" s="1">
         <v>3</v>
@@ -3756,7 +3757,7 @@
         <v>10</v>
       </c>
       <c r="G59" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="H59" s="5">
         <v>100000</v>
@@ -3775,7 +3776,7 @@
         <v>12</v>
       </c>
       <c r="M59" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="N59" t="str">
         <f t="shared" si="3"/>
@@ -3787,10 +3788,10 @@
         <v>59</v>
       </c>
       <c r="C60" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="D60" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="E60" s="1">
         <v>3</v>
@@ -3799,7 +3800,7 @@
         <v>10</v>
       </c>
       <c r="G60" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="H60" s="5">
         <v>250000</v>
@@ -3818,7 +3819,7 @@
         <v>12</v>
       </c>
       <c r="M60" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="N60" t="str">
         <f t="shared" si="3"/>
@@ -3830,10 +3831,10 @@
         <v>60</v>
       </c>
       <c r="C61" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="D61" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="E61" s="1">
         <v>4</v>
@@ -3842,7 +3843,7 @@
         <v>10</v>
       </c>
       <c r="G61" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="H61" s="5">
         <v>19000</v>
@@ -3861,7 +3862,7 @@
         <v>12</v>
       </c>
       <c r="M61" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="N61" t="str">
         <f t="shared" si="3"/>
@@ -3873,10 +3874,10 @@
         <v>61</v>
       </c>
       <c r="C62" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="D62" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="E62" s="1">
         <v>4</v>
@@ -3885,7 +3886,7 @@
         <v>10</v>
       </c>
       <c r="G62" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="H62" s="5">
         <v>191500</v>
@@ -3904,7 +3905,7 @@
         <v>13</v>
       </c>
       <c r="M62" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="N62" t="str">
         <f t="shared" si="3"/>
@@ -3916,10 +3917,10 @@
         <v>62</v>
       </c>
       <c r="C63" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="D63" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="E63" s="1">
         <v>4</v>
@@ -3928,7 +3929,7 @@
         <v>10</v>
       </c>
       <c r="G63" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="H63" s="5">
         <v>140000</v>
@@ -3947,7 +3948,7 @@
         <v>13</v>
       </c>
       <c r="M63" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="N63" t="str">
         <f t="shared" si="3"/>
@@ -3959,7 +3960,7 @@
         <v>14</v>
       </c>
       <c r="M64" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="N64" t="str">
         <f t="shared" si="3"/>
@@ -3971,7 +3972,7 @@
         <v>14</v>
       </c>
       <c r="M65" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="N65" t="str">
         <f t="shared" si="3"/>
@@ -3983,7 +3984,7 @@
         <v>15</v>
       </c>
       <c r="M66" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="N66" t="str">
         <f t="shared" si="3"/>
@@ -3995,7 +3996,7 @@
         <v>15</v>
       </c>
       <c r="M67" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="N67" t="str">
         <f t="shared" si="3"/>
@@ -4007,7 +4008,7 @@
         <v>16</v>
       </c>
       <c r="M68" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="N68" t="str">
         <f t="shared" si="3"/>
@@ -4019,7 +4020,7 @@
         <v>16</v>
       </c>
       <c r="M69" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="N69" t="str">
         <f t="shared" si="3"/>
@@ -4031,7 +4032,7 @@
         <v>17</v>
       </c>
       <c r="M70" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="N70" t="str">
         <f t="shared" si="3"/>
@@ -4043,7 +4044,7 @@
         <v>17</v>
       </c>
       <c r="M71" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="N71" t="str">
         <f t="shared" si="3"/>
@@ -4055,7 +4056,7 @@
         <v>18</v>
       </c>
       <c r="M72" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="N72" t="str">
         <f t="shared" si="3"/>
@@ -4067,7 +4068,7 @@
         <v>18</v>
       </c>
       <c r="M73" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="N73" t="str">
         <f t="shared" si="3"/>
@@ -4079,7 +4080,7 @@
         <v>19</v>
       </c>
       <c r="M74" s="3" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="N74" t="str">
         <f t="shared" si="3"/>
@@ -4091,7 +4092,7 @@
         <v>20</v>
       </c>
       <c r="M75" s="3" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="N75" t="str">
         <f t="shared" si="3"/>
@@ -4103,7 +4104,7 @@
         <v>21</v>
       </c>
       <c r="M76" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="N76" t="str">
         <f t="shared" si="3"/>
@@ -4115,7 +4116,7 @@
         <v>22</v>
       </c>
       <c r="M77" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="N77" t="str">
         <f t="shared" si="3"/>
@@ -4127,7 +4128,7 @@
         <v>23</v>
       </c>
       <c r="M78" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="N78" t="str">
         <f t="shared" si="3"/>
@@ -4139,7 +4140,7 @@
         <v>24</v>
       </c>
       <c r="M79" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="N79" t="str">
         <f t="shared" si="3"/>
@@ -4151,7 +4152,7 @@
         <v>25</v>
       </c>
       <c r="M80" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="N80" t="str">
         <f t="shared" si="3"/>
@@ -4163,7 +4164,7 @@
         <v>26</v>
       </c>
       <c r="M81" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="N81" t="str">
         <f t="shared" si="3"/>
@@ -4175,7 +4176,7 @@
         <v>27</v>
       </c>
       <c r="M82" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="N82" t="str">
         <f t="shared" si="3"/>
@@ -4187,7 +4188,7 @@
         <v>28</v>
       </c>
       <c r="M83" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="N83" t="str">
         <f t="shared" si="3"/>
@@ -4199,7 +4200,7 @@
         <v>29</v>
       </c>
       <c r="M84" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="N84" t="str">
         <f t="shared" si="3"/>
@@ -4211,7 +4212,7 @@
         <v>30</v>
       </c>
       <c r="M85" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="N85" t="str">
         <f t="shared" si="3"/>
@@ -4223,7 +4224,7 @@
         <v>31</v>
       </c>
       <c r="M86" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="N86" t="str">
         <f t="shared" si="3"/>
@@ -4235,7 +4236,7 @@
         <v>32</v>
       </c>
       <c r="M87" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="N87" t="str">
         <f t="shared" si="3"/>
@@ -4247,7 +4248,7 @@
         <v>33</v>
       </c>
       <c r="M88" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="N88" t="str">
         <f t="shared" si="3"/>
@@ -4259,7 +4260,7 @@
         <v>34</v>
       </c>
       <c r="M89" s="3" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="N89" t="str">
         <f t="shared" si="3"/>
@@ -4271,7 +4272,7 @@
         <v>35</v>
       </c>
       <c r="M90" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="N90" t="str">
         <f t="shared" si="3"/>
@@ -4283,7 +4284,7 @@
         <v>36</v>
       </c>
       <c r="M91" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="N91" t="str">
         <f t="shared" si="3"/>
@@ -4295,7 +4296,7 @@
         <v>38</v>
       </c>
       <c r="M92" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="N92" t="str">
         <f t="shared" si="3"/>
@@ -4307,7 +4308,7 @@
         <v>38</v>
       </c>
       <c r="M93" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="N93" t="str">
         <f t="shared" si="3"/>
@@ -4319,7 +4320,7 @@
         <v>39</v>
       </c>
       <c r="M94" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="N94" t="str">
         <f t="shared" si="3"/>
@@ -4331,7 +4332,7 @@
         <v>39</v>
       </c>
       <c r="M95" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="N95" t="str">
         <f t="shared" ref="N95:N137" si="4">CONCATENATE("INSERT INTO IMAGENES (idArticulo,  urlImagen) VALUES ('", L95, "','", TEXT(M95,"0"), "');")</f>
@@ -4343,7 +4344,7 @@
         <v>40</v>
       </c>
       <c r="M96" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="N96" t="str">
         <f t="shared" si="4"/>
@@ -4355,7 +4356,7 @@
         <v>40</v>
       </c>
       <c r="M97" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="N97" t="str">
         <f t="shared" si="4"/>
@@ -4367,7 +4368,7 @@
         <v>41</v>
       </c>
       <c r="M98" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="N98" t="str">
         <f t="shared" si="4"/>
@@ -4379,7 +4380,7 @@
         <v>41</v>
       </c>
       <c r="M99" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="N99" t="str">
         <f t="shared" si="4"/>
@@ -4391,7 +4392,7 @@
         <v>42</v>
       </c>
       <c r="M100" s="3" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="N100" t="str">
         <f t="shared" si="4"/>
@@ -4403,7 +4404,7 @@
         <v>42</v>
       </c>
       <c r="M101" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="N101" t="str">
         <f t="shared" si="4"/>
@@ -4415,7 +4416,7 @@
         <v>43</v>
       </c>
       <c r="M102" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="N102" t="str">
         <f t="shared" si="4"/>
@@ -4427,7 +4428,7 @@
         <v>43</v>
       </c>
       <c r="M103" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="N103" t="str">
         <f t="shared" si="4"/>
@@ -4439,7 +4440,7 @@
         <v>43</v>
       </c>
       <c r="M104" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="N104" t="str">
         <f t="shared" si="4"/>
@@ -4451,7 +4452,7 @@
         <v>44</v>
       </c>
       <c r="M105" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="N105" t="str">
         <f t="shared" si="4"/>
@@ -4463,7 +4464,7 @@
         <v>44</v>
       </c>
       <c r="M106" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="N106" t="str">
         <f t="shared" si="4"/>
@@ -4475,7 +4476,7 @@
         <v>45</v>
       </c>
       <c r="M107" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="N107" t="str">
         <f t="shared" si="4"/>
@@ -4487,7 +4488,7 @@
         <v>45</v>
       </c>
       <c r="M108" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="N108" t="str">
         <f t="shared" si="4"/>
@@ -4499,7 +4500,7 @@
         <v>46</v>
       </c>
       <c r="M109" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="N109" t="str">
         <f t="shared" si="4"/>
@@ -4511,7 +4512,7 @@
         <v>46</v>
       </c>
       <c r="M110" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="N110" t="str">
         <f t="shared" si="4"/>
@@ -4523,7 +4524,7 @@
         <v>47</v>
       </c>
       <c r="M111" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="N111" t="str">
         <f t="shared" si="4"/>
@@ -4535,7 +4536,7 @@
         <v>47</v>
       </c>
       <c r="M112" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="N112" t="str">
         <f t="shared" si="4"/>
@@ -4547,7 +4548,7 @@
         <v>48</v>
       </c>
       <c r="M113" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="N113" t="str">
         <f t="shared" si="4"/>
@@ -4559,7 +4560,7 @@
         <v>48</v>
       </c>
       <c r="M114" s="3" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="N114" t="str">
         <f t="shared" si="4"/>
@@ -4571,7 +4572,7 @@
         <v>49</v>
       </c>
       <c r="M115" s="3" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="N115" t="str">
         <f t="shared" si="4"/>
@@ -4583,7 +4584,7 @@
         <v>49</v>
       </c>
       <c r="M116" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="N116" t="str">
         <f t="shared" si="4"/>
@@ -4595,7 +4596,7 @@
         <v>50</v>
       </c>
       <c r="M117" s="3" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="N117" t="str">
         <f t="shared" si="4"/>
@@ -4607,7 +4608,7 @@
         <v>50</v>
       </c>
       <c r="M118" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="N118" t="str">
         <f t="shared" si="4"/>
@@ -4619,7 +4620,7 @@
         <v>51</v>
       </c>
       <c r="M119" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="N119" t="str">
         <f t="shared" si="4"/>
@@ -4631,7 +4632,7 @@
         <v>51</v>
       </c>
       <c r="M120" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="N120" t="str">
         <f t="shared" si="4"/>
@@ -4643,7 +4644,7 @@
         <v>52</v>
       </c>
       <c r="M121" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="N121" t="str">
         <f t="shared" si="4"/>
@@ -4655,7 +4656,7 @@
         <v>52</v>
       </c>
       <c r="M122" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="N122" t="str">
         <f t="shared" si="4"/>
@@ -4667,7 +4668,7 @@
         <v>53</v>
       </c>
       <c r="M123" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="N123" t="str">
         <f t="shared" si="4"/>
@@ -4679,7 +4680,7 @@
         <v>53</v>
       </c>
       <c r="M124" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="N124" t="str">
         <f t="shared" si="4"/>
@@ -4691,7 +4692,7 @@
         <v>54</v>
       </c>
       <c r="M125" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="N125" t="str">
         <f t="shared" si="4"/>
@@ -4703,7 +4704,7 @@
         <v>54</v>
       </c>
       <c r="M126" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="N126" t="str">
         <f t="shared" si="4"/>
@@ -4715,7 +4716,7 @@
         <v>55</v>
       </c>
       <c r="M127" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="N127" t="str">
         <f t="shared" si="4"/>
@@ -4727,7 +4728,7 @@
         <v>55</v>
       </c>
       <c r="M128" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="N128" t="str">
         <f t="shared" si="4"/>
@@ -4739,7 +4740,7 @@
         <v>56</v>
       </c>
       <c r="M129" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="N129" t="str">
         <f t="shared" si="4"/>
@@ -4751,7 +4752,7 @@
         <v>56</v>
       </c>
       <c r="M130" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="N130" t="str">
         <f t="shared" si="4"/>
@@ -4763,7 +4764,7 @@
         <v>57</v>
       </c>
       <c r="M131" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="N131" t="str">
         <f t="shared" si="4"/>
@@ -4775,7 +4776,7 @@
         <v>57</v>
       </c>
       <c r="M132" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="N132" t="str">
         <f t="shared" si="4"/>
@@ -4787,7 +4788,7 @@
         <v>58</v>
       </c>
       <c r="M133" s="3" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="N133" t="str">
         <f t="shared" si="4"/>
@@ -4799,7 +4800,7 @@
         <v>59</v>
       </c>
       <c r="M134" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="N134" t="str">
         <f t="shared" si="4"/>
@@ -4811,7 +4812,7 @@
         <v>60</v>
       </c>
       <c r="M135" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="N135" t="str">
         <f t="shared" si="4"/>
@@ -4823,7 +4824,7 @@
         <v>61</v>
       </c>
       <c r="M136" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="N136" t="str">
         <f t="shared" si="4"/>
@@ -4835,7 +4836,7 @@
         <v>62</v>
       </c>
       <c r="M137" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="N137" t="str">
         <f t="shared" si="4"/>
@@ -4844,45 +4845,36 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N18" r:id="rId1" xr:uid="{65F6FC56-4EFA-4C99-9163-0A1987B7A0F7}"/>
-    <hyperlink ref="N17" r:id="rId2" xr:uid="{90BABC38-EDC2-445C-8B49-B0BAE54D9632}"/>
-    <hyperlink ref="N21" r:id="rId3" xr:uid="{552F952D-A290-4373-B213-64FBE7D94BC5}"/>
-    <hyperlink ref="N23" r:id="rId4" xr:uid="{B419543B-8B5E-4F23-8D64-6D6E5FACBD3C}"/>
-    <hyperlink ref="N20" r:id="rId5" xr:uid="{B2E478FF-0E58-45C7-8C25-7E9306614484}"/>
-    <hyperlink ref="N15" r:id="rId6" xr:uid="{A6E49E6E-FC46-49A6-BDCC-3241FD8DD9C3}"/>
-    <hyperlink ref="N16" r:id="rId7" xr:uid="{7DCF332C-0794-4BA8-953D-0C029B2D35F9}"/>
-    <hyperlink ref="N19" r:id="rId8" xr:uid="{9703500F-BAC9-45E2-B946-044F6E61180B}"/>
-    <hyperlink ref="N2" r:id="rId9" xr:uid="{10C9DF36-12B2-4F5F-A5DA-DA91FE3B0BAF}"/>
-    <hyperlink ref="N3" r:id="rId10" xr:uid="{9FA1068C-27CE-4383-8E11-2CF87721C9F1}"/>
-    <hyperlink ref="N4" r:id="rId11" xr:uid="{B473844E-EC48-4FB2-9F82-B53BD9CA8771}"/>
-    <hyperlink ref="N5" r:id="rId12" xr:uid="{D0CC7DEE-D313-47F0-B676-E811858B98F8}"/>
-    <hyperlink ref="N6" r:id="rId13" xr:uid="{D22CE198-BA43-4D3F-A8E5-0676AA17E097}"/>
-    <hyperlink ref="N7" r:id="rId14" xr:uid="{3DAC407F-003F-4BA1-9700-04600EA06D5F}"/>
-    <hyperlink ref="N8" r:id="rId15" xr:uid="{E09C07E1-5D55-4129-A577-F2052C9282F8}"/>
-    <hyperlink ref="N9" r:id="rId16" xr:uid="{2F4CA7F8-8E60-4B68-93E0-F5B6FCF80E37}"/>
-    <hyperlink ref="N10" r:id="rId17" xr:uid="{973B891A-BA7B-485C-ADFC-199B773B872C}"/>
-    <hyperlink ref="N11" r:id="rId18" xr:uid="{140C5AF0-C088-4F0B-848B-BD5A8B0FBF8F}"/>
-    <hyperlink ref="N24" r:id="rId19" xr:uid="{000F6D95-E2FB-4627-B55C-578AE281638F}"/>
-    <hyperlink ref="M30" r:id="rId20" xr:uid="{FD63DC34-5E0E-40D3-9A8A-302EAD886E4E}"/>
-    <hyperlink ref="M35" r:id="rId21" xr:uid="{51460015-C9B9-45F6-B38C-B4F7E6BC21A1}"/>
-    <hyperlink ref="M36" r:id="rId22" xr:uid="{B49E5374-4385-4191-9502-4E04BB072550}"/>
-    <hyperlink ref="M38" r:id="rId23" xr:uid="{BD7B889C-E9F4-449C-B18F-F7A3B9272111}"/>
-    <hyperlink ref="M39" r:id="rId24" xr:uid="{FA380C96-0927-47B0-BBB3-EA19C076CA50}"/>
-    <hyperlink ref="M40" r:id="rId25" xr:uid="{3F8EACA5-B0B8-48B9-809F-E0D3FB9B096A}"/>
-    <hyperlink ref="M41" r:id="rId26" xr:uid="{80DACA7E-53FC-4073-A1BB-3054B5970E43}"/>
-    <hyperlink ref="M53" r:id="rId27" xr:uid="{BEEDEF9B-A0F7-4004-BB90-24F150823FAF}"/>
-    <hyperlink ref="M55" r:id="rId28" xr:uid="{F710BB8D-2A22-4433-AF7E-0D29A4065FDD}"/>
-    <hyperlink ref="M57" r:id="rId29" xr:uid="{69009564-5FAC-45A5-9655-AE1EAF0ACF59}"/>
-    <hyperlink ref="M74" r:id="rId30" xr:uid="{A8E29782-D602-4A5F-961B-8D8683BC06AA}"/>
-    <hyperlink ref="M75" r:id="rId31" xr:uid="{5CB24B7D-D387-4621-B46A-B70FCED81378}"/>
-    <hyperlink ref="M89" r:id="rId32" xr:uid="{23D2698E-0E87-4F08-8889-518FD2726D30}"/>
-    <hyperlink ref="M100" r:id="rId33" xr:uid="{3998F4BB-0709-40B7-A1A3-4C08F7088C35}"/>
-    <hyperlink ref="M115" r:id="rId34" xr:uid="{E3FCDBCE-9487-4A33-9B65-32EFE67633CA}"/>
-    <hyperlink ref="M114" r:id="rId35" xr:uid="{D5DDDC2A-520F-42E6-BFBD-51E31C3F4252}"/>
-    <hyperlink ref="M117" r:id="rId36" xr:uid="{9FCEE5C0-A9B0-4DDC-82A8-3A8E542CD3C1}"/>
-    <hyperlink ref="M133" r:id="rId37" xr:uid="{37746B62-0D34-4748-B28E-146894C54F16}"/>
+    <hyperlink ref="N2" r:id="rId1" xr:uid="{10C9DF36-12B2-4F5F-A5DA-DA91FE3B0BAF}"/>
+    <hyperlink ref="N3" r:id="rId2" xr:uid="{9FA1068C-27CE-4383-8E11-2CF87721C9F1}"/>
+    <hyperlink ref="N4" r:id="rId3" xr:uid="{B473844E-EC48-4FB2-9F82-B53BD9CA8771}"/>
+    <hyperlink ref="N5" r:id="rId4" xr:uid="{D0CC7DEE-D313-47F0-B676-E811858B98F8}"/>
+    <hyperlink ref="N6" r:id="rId5" xr:uid="{D22CE198-BA43-4D3F-A8E5-0676AA17E097}"/>
+    <hyperlink ref="N7" r:id="rId6" xr:uid="{3DAC407F-003F-4BA1-9700-04600EA06D5F}"/>
+    <hyperlink ref="N8" r:id="rId7" xr:uid="{E09C07E1-5D55-4129-A577-F2052C9282F8}"/>
+    <hyperlink ref="N9" r:id="rId8" xr:uid="{2F4CA7F8-8E60-4B68-93E0-F5B6FCF80E37}"/>
+    <hyperlink ref="N10" r:id="rId9" xr:uid="{973B891A-BA7B-485C-ADFC-199B773B872C}"/>
+    <hyperlink ref="N11" r:id="rId10" xr:uid="{140C5AF0-C088-4F0B-848B-BD5A8B0FBF8F}"/>
+    <hyperlink ref="M30" r:id="rId11" xr:uid="{FD63DC34-5E0E-40D3-9A8A-302EAD886E4E}"/>
+    <hyperlink ref="M35" r:id="rId12" xr:uid="{51460015-C9B9-45F6-B38C-B4F7E6BC21A1}"/>
+    <hyperlink ref="M36" r:id="rId13" xr:uid="{B49E5374-4385-4191-9502-4E04BB072550}"/>
+    <hyperlink ref="M38" r:id="rId14" xr:uid="{BD7B889C-E9F4-449C-B18F-F7A3B9272111}"/>
+    <hyperlink ref="M39" r:id="rId15" xr:uid="{FA380C96-0927-47B0-BBB3-EA19C076CA50}"/>
+    <hyperlink ref="M40" r:id="rId16" xr:uid="{3F8EACA5-B0B8-48B9-809F-E0D3FB9B096A}"/>
+    <hyperlink ref="M41" r:id="rId17" xr:uid="{80DACA7E-53FC-4073-A1BB-3054B5970E43}"/>
+    <hyperlink ref="M53" r:id="rId18" xr:uid="{BEEDEF9B-A0F7-4004-BB90-24F150823FAF}"/>
+    <hyperlink ref="M55" r:id="rId19" xr:uid="{F710BB8D-2A22-4433-AF7E-0D29A4065FDD}"/>
+    <hyperlink ref="M57" r:id="rId20" xr:uid="{69009564-5FAC-45A5-9655-AE1EAF0ACF59}"/>
+    <hyperlink ref="M74" r:id="rId21" xr:uid="{A8E29782-D602-4A5F-961B-8D8683BC06AA}"/>
+    <hyperlink ref="M75" r:id="rId22" xr:uid="{5CB24B7D-D387-4621-B46A-B70FCED81378}"/>
+    <hyperlink ref="M89" r:id="rId23" xr:uid="{23D2698E-0E87-4F08-8889-518FD2726D30}"/>
+    <hyperlink ref="M100" r:id="rId24" xr:uid="{3998F4BB-0709-40B7-A1A3-4C08F7088C35}"/>
+    <hyperlink ref="M115" r:id="rId25" xr:uid="{E3FCDBCE-9487-4A33-9B65-32EFE67633CA}"/>
+    <hyperlink ref="M114" r:id="rId26" xr:uid="{D5DDDC2A-520F-42E6-BFBD-51E31C3F4252}"/>
+    <hyperlink ref="M117" r:id="rId27" xr:uid="{9FCEE5C0-A9B0-4DDC-82A8-3A8E542CD3C1}"/>
+    <hyperlink ref="M133" r:id="rId28" xr:uid="{37746B62-0D34-4748-B28E-146894C54F16}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId38"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId29"/>
 </worksheet>
 </file>
</xml_diff>